<commit_message>
volver a subir el repusotorio con paths
</commit_message>
<xml_diff>
--- a/data/input/CLASIFICACION_ABC+D_MASCOTAS_VIVO_P1_2025.xlsx
+++ b/data/input/CLASIFICACION_ABC+D_MASCOTAS_VIVO_P1_2025.xlsx
@@ -12599,12 +12599,12 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2707100013</t>
+          <t>2707070003</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>NANACARA ANOMALA</t>
+          <t>TETRA PRISTELLA ROJA INIRIDA</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr"/>
@@ -12635,7 +12635,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>0</v>
@@ -12644,19 +12644,19 @@
         <v>0</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="P2" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R2" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S2" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T2" s="7" t="inlineStr">
         <is>
@@ -12665,12 +12665,12 @@
       </c>
       <c r="U2" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 44.1€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V2" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W2" s="4" t="inlineStr">
@@ -12682,36 +12682,28 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>2705040004</t>
+          <t>2204010007</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>PLANTAS EN TRONCO</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>3UD</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>CONEJO SUPER TOY PEDIGRI (ORYCTOLAGUS CUNICULUS)</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2204</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PEQUEÑOS MAMIFEROS</t>
         </is>
       </c>
       <c r="G3" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>0</v>
@@ -12741,10 +12733,10 @@
         <v>59</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R3" s="4" t="n">
-        <v>393.33</v>
+        <v>190</v>
       </c>
       <c r="S3" s="5" t="n">
         <v>30</v>
@@ -12756,12 +12748,12 @@
       </c>
       <c r="U3" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 12.35€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V3" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 02/01/2025</t>
         </is>
       </c>
       <c r="W3" s="4" t="inlineStr">
@@ -12773,12 +12765,12 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>2707100024</t>
+          <t>2707100004</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>APISTOGRAMA BORELLI</t>
+          <t>APISTOGRAMA CACATUOIDES</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr"/>
@@ -12824,10 +12816,10 @@
         <v>59</v>
       </c>
       <c r="Q4" s="4" t="n">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="R4" s="4" t="n">
-        <v>313.33</v>
+        <v>393.33</v>
       </c>
       <c r="S4" s="5" t="n">
         <v>30</v>
@@ -12839,12 +12831,12 @@
       </c>
       <c r="U4" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.79€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V4" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W4" s="4" t="inlineStr">
@@ -12856,24 +12848,24 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>2707100028</t>
+          <t>2806030001</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>PARACHROMIS MOTAGUENSIS 8-11 (CICLIDO JAGUAR ROJO)</t>
+          <t>COMETA SURTIDO XXL</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="3" t="inlineStr"/>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G5" s="4" t="n">
@@ -12892,7 +12884,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>0</v>
@@ -12901,7 +12893,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="P5" s="4" t="n">
         <v>59</v>
@@ -12922,7 +12914,7 @@
       </c>
       <c r="U5" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.57€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 51.56€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V5" s="4" t="inlineStr">
@@ -12939,12 +12931,12 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>2705040010</t>
+          <t>2705040009</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>BAMBU PIRAMIDE</t>
+          <t>HELECHO EN COCO PEQUEÑO</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr"/>
@@ -12975,7 +12967,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>0</v>
@@ -12984,7 +12976,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6" s="4" t="n">
         <v>59</v>
@@ -13005,7 +12997,7 @@
       </c>
       <c r="U6" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.98€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.52€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V6" s="4" t="inlineStr">
@@ -13022,12 +13014,12 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>2707120009</t>
+          <t>2707110001</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>LORICARIA FILAMENTOSA</t>
+          <t>BOTIA CARA CABALLO</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr"/>
@@ -13058,7 +13050,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M7" s="5" t="n">
         <v>0</v>
@@ -13067,7 +13059,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P7" s="4" t="n">
         <v>59</v>
@@ -13088,7 +13080,7 @@
       </c>
       <c r="U7" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 19.74€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.54€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V7" s="4" t="inlineStr">
@@ -13105,12 +13097,12 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>2707040007</t>
+          <t>2707100029</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>BARBO SAWBWA</t>
+          <t>RAMIREZI GOLD</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
@@ -13141,7 +13133,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M8" s="5" t="n">
         <v>0</v>
@@ -13150,19 +13142,19 @@
         <v>0</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P8" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q8" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R8" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S8" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T8" s="7" t="inlineStr">
         <is>
@@ -13171,12 +13163,12 @@
       </c>
       <c r="U8" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.59€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V8" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W8" s="4" t="inlineStr">
@@ -13188,16 +13180,24 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>2806030007</t>
+          <t>2806030001</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>SHUBUNKIN</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr"/>
-      <c r="D9" s="3" t="inlineStr"/>
+          <t>COMETA SURTIDO XXL</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>15CM</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
           <t>2806</t>
@@ -13224,7 +13224,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M9" s="5" t="n">
         <v>0</v>
@@ -13233,7 +13233,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P9" s="4" t="n">
         <v>59</v>
@@ -13254,7 +13254,7 @@
       </c>
       <c r="U9" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.22€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V9" s="4" t="inlineStr">
@@ -13271,28 +13271,28 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>2805040003</t>
+          <t>2707100002</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>PLANTA FLOTANTE MINI</t>
+          <t>ANDINOACARA PULCHER AZUL ELECTRICO 3-4</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr"/>
       <c r="D10" s="3" t="inlineStr"/>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>PLANTAS JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G10" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H10" s="4" t="n">
         <v>0</v>
@@ -13307,7 +13307,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>0</v>
@@ -13316,16 +13316,16 @@
         <v>0</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="P10" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="R10" s="4" t="n">
-        <v>173.33</v>
+        <v>393.33</v>
       </c>
       <c r="S10" s="5" t="n">
         <v>30</v>
@@ -13337,12 +13337,12 @@
       </c>
       <c r="U10" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.47€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V10" s="4" t="inlineStr">
         <is>
-          <t>Compra 07/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W10" s="4" t="inlineStr">
@@ -13354,12 +13354,12 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>2707100016</t>
+          <t>2707130082</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI ALEMAN AZUL (MIKROGEOPHAGUS)</t>
+          <t>RASBORA VERDE NEON</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr"/>
@@ -13390,7 +13390,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="M11" s="5" t="n">
         <v>0</v>
@@ -13399,16 +13399,16 @@
         <v>0</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="P11" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q11" s="4" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="R11" s="4" t="n">
-        <v>220</v>
+        <v>393.33</v>
       </c>
       <c r="S11" s="5" t="n">
         <v>30</v>
@@ -13420,12 +13420,12 @@
       </c>
       <c r="U11" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V11" s="4" t="inlineStr">
         <is>
-          <t>Compra 26/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W11" s="4" t="inlineStr">
@@ -13437,32 +13437,24 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>2806030001</t>
+          <t>2707110005</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>COMETA SURTIDO XXL</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>15CM</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BOTIA MORLETI 4</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr"/>
+      <c r="D12" s="3" t="inlineStr"/>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G12" s="4" t="n">
@@ -13481,7 +13473,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M12" s="5" t="n">
         <v>0</v>
@@ -13490,7 +13482,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="4" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="P12" s="4" t="n">
         <v>59</v>
@@ -13511,7 +13503,7 @@
       </c>
       <c r="U12" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.22€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V12" s="4" t="inlineStr">
@@ -13528,28 +13520,28 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>2707090002</t>
+          <t>2104080003</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>CICLIDO TANGANICA SURTIDO</t>
+          <t>PERIQUITO INGLES (MELOPSITTACUS UNDULATUS)</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr"/>
       <c r="D13" s="3" t="inlineStr"/>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G13" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H13" s="4" t="n">
         <v>0</v>
@@ -13564,7 +13556,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M13" s="5" t="n">
         <v>0</v>
@@ -13573,7 +13565,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P13" s="4" t="n">
         <v>59</v>
@@ -13582,7 +13574,7 @@
         <v>59</v>
       </c>
       <c r="R13" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S13" s="5" t="n">
         <v>30</v>
@@ -13594,7 +13586,7 @@
       </c>
       <c r="U13" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.9€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 67.2€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V13" s="4" t="inlineStr">
@@ -13611,12 +13603,12 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>2707130018</t>
+          <t>2707130054</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>GARRA RUFA ARCOIRIS FLAVATRA</t>
+          <t>PEZ CUCHILLO PAYASO</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr"/>
@@ -13647,7 +13639,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M14" s="5" t="n">
         <v>0</v>
@@ -13656,7 +13648,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P14" s="4" t="n">
         <v>59</v>
@@ -13677,7 +13669,7 @@
       </c>
       <c r="U14" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.56€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.09€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V14" s="4" t="inlineStr">
@@ -13694,36 +13686,28 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>2708010010</t>
+          <t>2606050000</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>FANTAIL SURTIDO</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>5CM</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BICHO PALO</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2606</t>
         </is>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>ANIMAL VIVO REPTILES</t>
         </is>
       </c>
       <c r="G15" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H15" s="4" t="n">
         <v>0</v>
@@ -13738,7 +13722,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>0</v>
@@ -13747,16 +13731,16 @@
         <v>0</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="P15" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q15" s="4" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="R15" s="4" t="n">
-        <v>53.33</v>
+        <v>63.33</v>
       </c>
       <c r="S15" s="5" t="n">
         <v>0</v>
@@ -13773,7 +13757,7 @@
       </c>
       <c r="V15" s="4" t="inlineStr">
         <is>
-          <t>Compra 20/02/2025</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W15" s="4" t="inlineStr">
@@ -13785,12 +13769,12 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>2707100004</t>
+          <t>2707100016</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>APISTOGRAMA CACATUOIDES</t>
+          <t>RAMIREZI ALEMAN AZUL (MIKROGEOPHAGUS)</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
@@ -13821,7 +13805,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M16" s="5" t="n">
         <v>0</v>
@@ -13830,16 +13814,16 @@
         <v>0</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P16" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q16" s="4" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="R16" s="4" t="n">
-        <v>393.33</v>
+        <v>220</v>
       </c>
       <c r="S16" s="5" t="n">
         <v>30</v>
@@ -13851,12 +13835,12 @@
       </c>
       <c r="U16" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.79€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V16" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 26/01/2025</t>
         </is>
       </c>
       <c r="W16" s="4" t="inlineStr">
@@ -13868,28 +13852,28 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>2708020003</t>
+          <t>2104080001</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>ORANDA SURTIDO</t>
+          <t>PERIQUITO BURQUE</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr"/>
       <c r="D17" s="3" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G17" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H17" s="4" t="n">
         <v>0</v>
@@ -13904,7 +13888,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="M17" s="5" t="n">
         <v>0</v>
@@ -13913,7 +13897,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="P17" s="4" t="n">
         <v>59</v>
@@ -13922,7 +13906,7 @@
         <v>59</v>
       </c>
       <c r="R17" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S17" s="5" t="n">
         <v>30</v>
@@ -13934,7 +13918,7 @@
       </c>
       <c r="U17" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 59.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 24.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V17" s="4" t="inlineStr">
@@ -13951,24 +13935,24 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>2707090010</t>
+          <t>2708010019</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>KANDANGO ROJO</t>
+          <t>CABEZA DE LEON</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr"/>
       <c r="D18" s="3" t="inlineStr"/>
       <c r="E18" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G18" s="4" t="n">
@@ -14002,13 +13986,13 @@
         <v>59</v>
       </c>
       <c r="Q18" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R18" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S18" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T18" s="7" t="inlineStr">
         <is>
@@ -14017,12 +14001,12 @@
       </c>
       <c r="U18" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.29€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V18" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W18" s="4" t="inlineStr">
@@ -14034,12 +14018,12 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>2707130035</t>
+          <t>2707130083</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>PEZ HACHA</t>
+          <t>POPONDETA PASKAI</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr"/>
@@ -14070,7 +14054,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M19" s="5" t="n">
         <v>0</v>
@@ -14079,16 +14063,16 @@
         <v>0</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P19" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q19" s="4" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="R19" s="4" t="n">
-        <v>393.33</v>
+        <v>313.33</v>
       </c>
       <c r="S19" s="5" t="n">
         <v>30</v>
@@ -14100,12 +14084,12 @@
       </c>
       <c r="U19" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.18€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V19" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W19" s="4" t="inlineStr">
@@ -14117,12 +14101,12 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>2707120007</t>
+          <t>2707170006</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>PANAQUE REAL L190</t>
+          <t>BADIS ESCARLATA</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr"/>
@@ -14153,7 +14137,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="M20" s="5" t="n">
         <v>0</v>
@@ -14162,7 +14146,7 @@
         <v>0</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="P20" s="4" t="n">
         <v>59</v>
@@ -14183,7 +14167,7 @@
       </c>
       <c r="U20" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.72€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.48€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V20" s="4" t="inlineStr">
@@ -14200,24 +14184,24 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>2707110005</t>
+          <t>2708010014</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>BOTIA MORLETI 4</t>
+          <t>RYUKIN SURTIDO</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr"/>
       <c r="D21" s="3" t="inlineStr"/>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G21" s="4" t="n">
@@ -14236,7 +14220,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M21" s="5" t="n">
         <v>0</v>
@@ -14245,7 +14229,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P21" s="4" t="n">
         <v>59</v>
@@ -14266,7 +14250,7 @@
       </c>
       <c r="U21" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 31.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V21" s="4" t="inlineStr">
@@ -14283,28 +14267,28 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>2104090006</t>
+          <t>2707050001</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>FORPUS MUTACION AZUL (FORPUS COELESTIS)</t>
+          <t>BESUCON HELOSTOMA TEMMINCKII</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr"/>
       <c r="D22" s="3" t="inlineStr"/>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G22" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H22" s="4" t="n">
         <v>0</v>
@@ -14319,7 +14303,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M22" s="5" t="n">
         <v>0</v>
@@ -14328,19 +14312,19 @@
         <v>0</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P22" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q22" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R22" s="4" t="n">
-        <v>196.67</v>
+        <v>33.33</v>
       </c>
       <c r="S22" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T22" s="7" t="inlineStr">
         <is>
@@ -14349,12 +14333,12 @@
       </c>
       <c r="U22" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V22" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W22" s="4" t="inlineStr">
@@ -14366,24 +14350,32 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>2705040006</t>
+          <t>2707110006</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>ANUBIA MIX COCO HALF</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="inlineStr"/>
-      <c r="D23" s="3" t="inlineStr"/>
+          <t>BOTIA PAYASO</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>7CM</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G23" s="4" t="n">
@@ -14402,7 +14394,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="4" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M23" s="5" t="n">
         <v>0</v>
@@ -14411,7 +14403,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="4" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="P23" s="4" t="n">
         <v>59</v>
@@ -14432,7 +14424,7 @@
       </c>
       <c r="U23" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 57.24€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.91€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V23" s="4" t="inlineStr">
@@ -14449,24 +14441,24 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>2204010007</t>
+          <t>2104090002</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>CONEJO SUPER TOY PEDIGRI (ORYCTOLAGUS CUNICULUS)</t>
+          <t>DIAMANTE BICHENOW (POEPHILA BICHENOVII) DIABI</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr"/>
       <c r="D24" s="3" t="inlineStr"/>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>2204</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PEQUEÑOS MAMIFEROS</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G24" s="4" t="n">
@@ -14500,10 +14492,10 @@
         <v>59</v>
       </c>
       <c r="Q24" s="4" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R24" s="4" t="n">
-        <v>190</v>
+        <v>196.67</v>
       </c>
       <c r="S24" s="5" t="n">
         <v>30</v>
@@ -14515,12 +14507,12 @@
       </c>
       <c r="U24" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V24" s="4" t="inlineStr">
         <is>
-          <t>Compra 02/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W24" s="4" t="inlineStr">
@@ -14532,12 +14524,12 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>2707100040</t>
+          <t>2707120007</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI BOLIVIANO (PAPILIOCHROMIS ALTISPINOSA)</t>
+          <t>PANAQUE REAL L190</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr"/>
@@ -14568,7 +14560,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M25" s="5" t="n">
         <v>0</v>
@@ -14577,16 +14569,16 @@
         <v>0</v>
       </c>
       <c r="O25" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P25" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q25" s="4" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="R25" s="4" t="n">
-        <v>220</v>
+        <v>393.33</v>
       </c>
       <c r="S25" s="5" t="n">
         <v>30</v>
@@ -14598,12 +14590,12 @@
       </c>
       <c r="U25" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.72€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V25" s="4" t="inlineStr">
         <is>
-          <t>Compra 26/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W25" s="4" t="inlineStr">
@@ -14615,12 +14607,12 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>2707110022</t>
+          <t>2707130079</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>CORYDORA ORANGE VENEZUELA</t>
+          <t>GOBIO PAVO REAL</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr"/>
@@ -14651,7 +14643,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M26" s="5" t="n">
         <v>0</v>
@@ -14660,7 +14652,7 @@
         <v>0</v>
       </c>
       <c r="O26" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P26" s="4" t="n">
         <v>59</v>
@@ -14681,7 +14673,7 @@
       </c>
       <c r="U26" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 9.58€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.97€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V26" s="4" t="inlineStr">
@@ -14698,12 +14690,12 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>2705040003</t>
+          <t>2705040010</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA XL</t>
+          <t>BAMBU PIRAMIDE</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr"/>
@@ -14734,7 +14726,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M27" s="5" t="n">
         <v>0</v>
@@ -14743,7 +14735,7 @@
         <v>0</v>
       </c>
       <c r="O27" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P27" s="4" t="n">
         <v>59</v>
@@ -14764,7 +14756,7 @@
       </c>
       <c r="U27" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.29€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.98€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V27" s="4" t="inlineStr">
@@ -14781,12 +14773,12 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>2707110023</t>
+          <t>2707050019</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>BOTIA SUMO</t>
+          <t>PEZ PARAISO MACROPODUS</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr"/>
@@ -14847,7 +14839,7 @@
       </c>
       <c r="U28" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.96€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V28" s="4" t="inlineStr">
@@ -14864,12 +14856,12 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>2707130021</t>
+          <t>2707170002</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>MELANOTAENIA SURTIDO</t>
+          <t>PEZ SIERRA SELECTO</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr"/>
@@ -14900,7 +14892,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M29" s="5" t="n">
         <v>0</v>
@@ -14909,19 +14901,19 @@
         <v>0</v>
       </c>
       <c r="O29" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P29" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q29" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R29" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S29" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T29" s="7" t="inlineStr">
         <is>
@@ -14930,12 +14922,12 @@
       </c>
       <c r="U29" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.15€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V29" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W29" s="4" t="inlineStr">
@@ -14947,12 +14939,12 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>2707050022</t>
+          <t>2707080006</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>BETTA KOI</t>
+          <t>ESCALAR RED DEVIL</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr"/>
@@ -14983,7 +14975,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M30" s="5" t="n">
         <v>0</v>
@@ -14992,19 +14984,19 @@
         <v>0</v>
       </c>
       <c r="O30" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="P30" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q30" s="4" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="R30" s="4" t="n">
-        <v>126.67</v>
+        <v>33.33</v>
       </c>
       <c r="S30" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T30" s="7" t="inlineStr">
         <is>
@@ -15013,12 +15005,12 @@
       </c>
       <c r="U30" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V30" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W30" s="4" t="inlineStr">
@@ -15030,12 +15022,12 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>2707050028</t>
+          <t>2707100013</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>BETTA HELLBOY MACHO</t>
+          <t>NANACARA ANOMALA</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr"/>
@@ -15066,7 +15058,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M31" s="5" t="n">
         <v>0</v>
@@ -15075,19 +15067,19 @@
         <v>0</v>
       </c>
       <c r="O31" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P31" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q31" s="4" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="R31" s="4" t="n">
-        <v>33.33</v>
+        <v>126.67</v>
       </c>
       <c r="S31" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T31" s="7" t="inlineStr">
         <is>
@@ -15096,12 +15088,12 @@
       </c>
       <c r="U31" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V31" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W31" s="4" t="inlineStr">
@@ -15113,12 +15105,12 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>2707110001</t>
+          <t>2707130035</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>BOTIA CARA CABALLO</t>
+          <t>PEZ HACHA</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr"/>
@@ -15149,7 +15141,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M32" s="5" t="n">
         <v>0</v>
@@ -15158,7 +15150,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P32" s="4" t="n">
         <v>59</v>
@@ -15179,7 +15171,7 @@
       </c>
       <c r="U32" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.54€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.18€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V32" s="4" t="inlineStr">
@@ -15196,28 +15188,28 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>2104090002</t>
+          <t>2707090009</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>DIAMANTE BICHENOW (POEPHILA BICHENOVII) DIABI</t>
+          <t>AULONOCARA CALICO RED NEON</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr"/>
       <c r="D33" s="3" t="inlineStr"/>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F33" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G33" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H33" s="4" t="n">
         <v>0</v>
@@ -15232,7 +15224,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M33" s="5" t="n">
         <v>0</v>
@@ -15241,7 +15233,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P33" s="4" t="n">
         <v>59</v>
@@ -15250,7 +15242,7 @@
         <v>59</v>
       </c>
       <c r="R33" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S33" s="5" t="n">
         <v>30</v>
@@ -15262,7 +15254,7 @@
       </c>
       <c r="U33" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V33" s="4" t="inlineStr">
@@ -15279,24 +15271,24 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>2806030001</t>
+          <t>2707100040</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>COMETA SURTIDO XXL</t>
+          <t>RAMIREZI BOLIVIANO (PAPILIOCHROMIS ALTISPINOSA)</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr"/>
       <c r="D34" s="3" t="inlineStr"/>
       <c r="E34" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F34" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G34" s="4" t="n">
@@ -15315,7 +15307,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="4" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="M34" s="5" t="n">
         <v>0</v>
@@ -15324,16 +15316,16 @@
         <v>0</v>
       </c>
       <c r="O34" s="4" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="P34" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q34" s="4" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="R34" s="4" t="n">
-        <v>393.33</v>
+        <v>220</v>
       </c>
       <c r="S34" s="5" t="n">
         <v>30</v>
@@ -15345,12 +15337,12 @@
       </c>
       <c r="U34" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 51.56€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V34" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 26/01/2025</t>
         </is>
       </c>
       <c r="W34" s="4" t="inlineStr">
@@ -15362,12 +15354,12 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>2707190007</t>
+          <t>2707110022</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>PANAQUE MAMLUS L104</t>
+          <t>CORYDORA ORANGE VENEZUELA</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr"/>
@@ -15398,7 +15390,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M35" s="5" t="n">
         <v>0</v>
@@ -15407,7 +15399,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P35" s="4" t="n">
         <v>59</v>
@@ -15428,7 +15420,7 @@
       </c>
       <c r="U35" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 21.39€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 9.58€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V35" s="4" t="inlineStr">
@@ -15445,12 +15437,12 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>2707050019</t>
+          <t>2707130041</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>PEZ PARAISO MACROPODUS</t>
+          <t>POPONDETA FURCATA</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr"/>
@@ -15511,7 +15503,7 @@
       </c>
       <c r="U36" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.96€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V36" s="4" t="inlineStr">
@@ -15528,12 +15520,12 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>2707130047</t>
+          <t>2707120003</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>RASBORA MACULATUS</t>
+          <t>LORICARIA SP RED</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr"/>
@@ -15564,7 +15556,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="4" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="M37" s="5" t="n">
         <v>0</v>
@@ -15573,7 +15565,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="4" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="P37" s="4" t="n">
         <v>59</v>
@@ -15594,7 +15586,7 @@
       </c>
       <c r="U37" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.3€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V37" s="4" t="inlineStr">
@@ -15611,28 +15603,28 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>2707130079</t>
+          <t>2104090001</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>GOBIO PAVO REAL</t>
+          <t>DIAMANTE BARBERO COLA LARGA</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr"/>
       <c r="D38" s="3" t="inlineStr"/>
       <c r="E38" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F38" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G38" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H38" s="4" t="n">
         <v>0</v>
@@ -15647,7 +15639,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M38" s="5" t="n">
         <v>0</v>
@@ -15656,7 +15648,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P38" s="4" t="n">
         <v>59</v>
@@ -15665,7 +15657,7 @@
         <v>59</v>
       </c>
       <c r="R38" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S38" s="5" t="n">
         <v>30</v>
@@ -15677,7 +15669,7 @@
       </c>
       <c r="U38" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.97€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V38" s="4" t="inlineStr">
@@ -15694,12 +15686,12 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>2707120001</t>
+          <t>2707040006</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>HYPANCISTRUS SP L333 5-6</t>
+          <t>BARBO ARCOIRIS (NOTROPIS CHROSOMUS)</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr"/>
@@ -15730,7 +15722,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="4" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="M39" s="5" t="n">
         <v>0</v>
@@ -15739,19 +15731,19 @@
         <v>0</v>
       </c>
       <c r="O39" s="4" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="P39" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q39" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R39" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S39" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T39" s="7" t="inlineStr">
         <is>
@@ -15760,12 +15752,12 @@
       </c>
       <c r="U39" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.64€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V39" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W39" s="4" t="inlineStr">
@@ -15777,12 +15769,12 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>2707130031</t>
+          <t>2707100028</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>PEZ DOLAR PLATA</t>
+          <t>PARACHROMIS MOTAGUENSIS 8-11 (CICLIDO JAGUAR ROJO)</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr"/>
@@ -15813,7 +15805,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M40" s="5" t="n">
         <v>0</v>
@@ -15822,7 +15814,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P40" s="4" t="n">
         <v>59</v>
@@ -15843,7 +15835,7 @@
       </c>
       <c r="U40" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.35€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.57€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V40" s="4" t="inlineStr">
@@ -15860,12 +15852,12 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>2707050021</t>
+          <t>2707130047</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>BESUCON BALON</t>
+          <t>RASBORA MACULATUS</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr"/>
@@ -15896,7 +15888,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="4" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="M41" s="5" t="n">
         <v>0</v>
@@ -15905,7 +15897,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="4" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="P41" s="4" t="n">
         <v>59</v>
@@ -15926,7 +15918,7 @@
       </c>
       <c r="U41" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.04€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V41" s="4" t="inlineStr">
@@ -15943,12 +15935,12 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>2707130084</t>
+          <t>2707130021</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>PANCHAX RAYADO</t>
+          <t>MELANOTAENIA SURTIDO</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr"/>
@@ -15994,13 +15986,13 @@
         <v>59</v>
       </c>
       <c r="Q42" s="4" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="R42" s="4" t="n">
-        <v>33.33</v>
+        <v>126.67</v>
       </c>
       <c r="S42" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T42" s="7" t="inlineStr">
         <is>
@@ -16009,12 +16001,12 @@
       </c>
       <c r="U42" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V42" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W42" s="4" t="inlineStr">
@@ -16026,24 +16018,24 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>2708010019</t>
+          <t>2707130020</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>CABEZA DE LEON</t>
+          <t>LABEO ZORRO VOLADOR</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr"/>
       <c r="D43" s="3" t="inlineStr"/>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F43" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G43" s="4" t="n">
@@ -16062,7 +16054,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="M43" s="5" t="n">
         <v>0</v>
@@ -16071,19 +16063,19 @@
         <v>0</v>
       </c>
       <c r="O43" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="P43" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q43" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R43" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S43" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T43" s="7" t="inlineStr">
         <is>
@@ -16092,12 +16084,12 @@
       </c>
       <c r="U43" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 8.32€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V43" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W43" s="4" t="inlineStr">
@@ -16109,12 +16101,12 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>2707130082</t>
+          <t>2707050021</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>RASBORA VERDE NEON</t>
+          <t>BESUCON BALON</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr"/>
@@ -16145,7 +16137,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="4" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="M44" s="5" t="n">
         <v>0</v>
@@ -16154,7 +16146,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="4" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="P44" s="4" t="n">
         <v>59</v>
@@ -16175,7 +16167,7 @@
       </c>
       <c r="U44" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.04€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V44" s="4" t="inlineStr">
@@ -16192,24 +16184,24 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>2705040008</t>
+          <t>2708020003</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>ANUBIA EN ROCA</t>
+          <t>ORANDA SURTIDO</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr"/>
       <c r="D45" s="3" t="inlineStr"/>
       <c r="E45" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F45" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G45" s="4" t="n">
@@ -16228,7 +16220,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="4" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="M45" s="5" t="n">
         <v>0</v>
@@ -16237,7 +16229,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="4" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="P45" s="4" t="n">
         <v>59</v>
@@ -16258,7 +16250,7 @@
       </c>
       <c r="U45" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.27€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 59.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V45" s="4" t="inlineStr">
@@ -16275,12 +16267,12 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>2707130006</t>
+          <t>2707100011</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>CRISTAL DE JAVA - BICHIRRI CRISTAL</t>
+          <t>HEROS SEVERUM</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr"/>
@@ -16311,7 +16303,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M46" s="5" t="n">
         <v>0</v>
@@ -16320,16 +16312,16 @@
         <v>0</v>
       </c>
       <c r="O46" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P46" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q46" s="4" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="R46" s="4" t="n">
-        <v>393.33</v>
+        <v>313.33</v>
       </c>
       <c r="S46" s="5" t="n">
         <v>30</v>
@@ -16341,12 +16333,12 @@
       </c>
       <c r="U46" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.33€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V46" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W46" s="4" t="inlineStr">
@@ -16358,12 +16350,12 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>2707130083</t>
+          <t>2707090002</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>POPONDETA PASKAI</t>
+          <t>CICLIDO TANGANICA SURTIDO</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr"/>
@@ -16394,7 +16386,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M47" s="5" t="n">
         <v>0</v>
@@ -16403,16 +16395,16 @@
         <v>0</v>
       </c>
       <c r="O47" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P47" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q47" s="4" t="n">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="R47" s="4" t="n">
-        <v>313.33</v>
+        <v>393.33</v>
       </c>
       <c r="S47" s="5" t="n">
         <v>30</v>
@@ -16424,12 +16416,12 @@
       </c>
       <c r="U47" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.9€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V47" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W47" s="4" t="inlineStr">
@@ -16441,12 +16433,12 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>2707130075</t>
+          <t>2707040007</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>PEZ MEDIO PICO BUFON (HEMIRHAMPHODON KUEKENTHALI)</t>
+          <t>BARBO SAWBWA</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr"/>
@@ -16477,7 +16469,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M48" s="5" t="n">
         <v>0</v>
@@ -16486,19 +16478,19 @@
         <v>0</v>
       </c>
       <c r="O48" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="P48" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q48" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R48" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S48" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T48" s="7" t="inlineStr">
         <is>
@@ -16507,12 +16499,12 @@
       </c>
       <c r="U48" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.26€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V48" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W48" s="4" t="inlineStr">
@@ -16524,24 +16516,24 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>2707040006</t>
+          <t>2705040011</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>BARBO ARCOIRIS (NOTROPIS CHROSOMUS)</t>
+          <t>BAMBU CUEVA</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr"/>
       <c r="D49" s="3" t="inlineStr"/>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F49" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G49" s="4" t="n">
@@ -16560,7 +16552,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="M49" s="5" t="n">
         <v>0</v>
@@ -16569,19 +16561,19 @@
         <v>0</v>
       </c>
       <c r="O49" s="4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P49" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q49" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R49" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S49" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T49" s="7" t="inlineStr">
         <is>
@@ -16590,12 +16582,12 @@
       </c>
       <c r="U49" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.32€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V49" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W49" s="4" t="inlineStr">
@@ -16607,12 +16599,12 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>2707130026</t>
+          <t>2707120009</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>PANGASIUS SUTCHI</t>
+          <t>LORICARIA FILAMENTOSA</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr"/>
@@ -16643,7 +16635,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M50" s="5" t="n">
         <v>0</v>
@@ -16652,7 +16644,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P50" s="4" t="n">
         <v>59</v>
@@ -16673,7 +16665,7 @@
       </c>
       <c r="U50" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.15€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 19.74€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V50" s="4" t="inlineStr">
@@ -16690,12 +16682,12 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>2707050001</t>
+          <t>2707130075</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>BESUCON HELOSTOMA TEMMINCKII</t>
+          <t>PEZ MEDIO PICO BUFON (HEMIRHAMPHODON KUEKENTHALI)</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr"/>
@@ -16726,7 +16718,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M51" s="5" t="n">
         <v>0</v>
@@ -16735,19 +16727,19 @@
         <v>0</v>
       </c>
       <c r="O51" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P51" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q51" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R51" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S51" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T51" s="7" t="inlineStr">
         <is>
@@ -16756,12 +16748,12 @@
       </c>
       <c r="U51" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.26€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V51" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W51" s="4" t="inlineStr">
@@ -16773,12 +16765,12 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>2707100002</t>
+          <t>2707100038</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>ANDINOACARA PULCHER AZUL ELECTRICO 3-4</t>
+          <t>RAMIREZI BLACK DEVIL</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr"/>
@@ -16809,7 +16801,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M52" s="5" t="n">
         <v>0</v>
@@ -16818,7 +16810,7 @@
         <v>0</v>
       </c>
       <c r="O52" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P52" s="4" t="n">
         <v>59</v>
@@ -16839,7 +16831,7 @@
       </c>
       <c r="U52" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.47€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 28.48€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V52" s="4" t="inlineStr">
@@ -16856,16 +16848,24 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>2707100029</t>
+          <t>2707130025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI GOLD</t>
-        </is>
-      </c>
-      <c r="C53" s="3" t="inlineStr"/>
-      <c r="D53" s="3" t="inlineStr"/>
+          <t>PANGASIUS ALBINO</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>6I7</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E53" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -16892,7 +16892,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M53" s="5" t="n">
         <v>0</v>
@@ -16901,7 +16901,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P53" s="4" t="n">
         <v>59</v>
@@ -16922,7 +16922,7 @@
       </c>
       <c r="U53" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.59€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.1€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V53" s="4" t="inlineStr">
@@ -16939,24 +16939,24 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>2707050026</t>
+          <t>2708010007</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>BETTA MACHO LONG TAIL</t>
+          <t>COMETA SARASA</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr"/>
       <c r="D54" s="3" t="inlineStr"/>
       <c r="E54" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F54" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G54" s="4" t="n">
@@ -16975,7 +16975,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M54" s="5" t="n">
         <v>0</v>
@@ -16984,7 +16984,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P54" s="4" t="n">
         <v>59</v>
@@ -17005,7 +17005,7 @@
       </c>
       <c r="U54" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.92€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.84€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V54" s="4" t="inlineStr">
@@ -17022,24 +17022,32 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>2707100011</t>
+          <t>2708010014</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>HEROS SEVERUM</t>
-        </is>
-      </c>
-      <c r="C55" s="3" t="inlineStr"/>
-      <c r="D55" s="3" t="inlineStr"/>
+          <t>RYUKIN SURTIDO</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="inlineStr">
+        <is>
+          <t>5I6</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F55" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G55" s="4" t="n">
@@ -17058,7 +17066,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M55" s="5" t="n">
         <v>0</v>
@@ -17067,16 +17075,16 @@
         <v>0</v>
       </c>
       <c r="O55" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P55" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q55" s="4" t="n">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="R55" s="4" t="n">
-        <v>313.33</v>
+        <v>380</v>
       </c>
       <c r="S55" s="5" t="n">
         <v>30</v>
@@ -17093,7 +17101,7 @@
       </c>
       <c r="V55" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Compra 02/01/2025</t>
         </is>
       </c>
       <c r="W55" s="4" t="inlineStr">
@@ -17105,32 +17113,24 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>2708010014</t>
+          <t>2705040003</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>RYUKIN SURTIDO</t>
-        </is>
-      </c>
-      <c r="C56" s="3" t="inlineStr">
-        <is>
-          <t>5I6</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>PLANTA ACUATICA XL</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="inlineStr"/>
+      <c r="D56" s="3" t="inlineStr"/>
       <c r="E56" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F56" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G56" s="4" t="n">
@@ -17149,7 +17149,7 @@
         <v>0</v>
       </c>
       <c r="L56" s="4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M56" s="5" t="n">
         <v>0</v>
@@ -17158,16 +17158,16 @@
         <v>0</v>
       </c>
       <c r="O56" s="4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="P56" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q56" s="4" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R56" s="4" t="n">
-        <v>380</v>
+        <v>393.33</v>
       </c>
       <c r="S56" s="5" t="n">
         <v>30</v>
@@ -17179,12 +17179,12 @@
       </c>
       <c r="U56" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.29€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V56" s="4" t="inlineStr">
         <is>
-          <t>Compra 02/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W56" s="4" t="inlineStr">
@@ -17196,12 +17196,12 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>2705040011</t>
+          <t>2705040006</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>BAMBU CUEVA</t>
+          <t>ANUBIA MIX COCO HALF</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr"/>
@@ -17232,7 +17232,7 @@
         <v>0</v>
       </c>
       <c r="L57" s="4" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="M57" s="5" t="n">
         <v>0</v>
@@ -17241,7 +17241,7 @@
         <v>0</v>
       </c>
       <c r="O57" s="4" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="P57" s="4" t="n">
         <v>59</v>
@@ -17262,7 +17262,7 @@
       </c>
       <c r="U57" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.32€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 57.24€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V57" s="4" t="inlineStr">
@@ -17279,28 +17279,28 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>2104090001</t>
+          <t>2707050026</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>DIAMANTE BARBERO COLA LARGA</t>
+          <t>BETTA MACHO LONG TAIL</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr"/>
       <c r="D58" s="3" t="inlineStr"/>
       <c r="E58" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G58" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H58" s="4" t="n">
         <v>0</v>
@@ -17315,7 +17315,7 @@
         <v>0</v>
       </c>
       <c r="L58" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M58" s="5" t="n">
         <v>0</v>
@@ -17324,7 +17324,7 @@
         <v>0</v>
       </c>
       <c r="O58" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P58" s="4" t="n">
         <v>59</v>
@@ -17333,7 +17333,7 @@
         <v>59</v>
       </c>
       <c r="R58" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S58" s="5" t="n">
         <v>30</v>
@@ -17345,7 +17345,7 @@
       </c>
       <c r="U58" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.92€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V58" s="4" t="inlineStr">
@@ -17362,24 +17362,24 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>2708010014</t>
+          <t>2707130018</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>RYUKIN SURTIDO</t>
+          <t>GARRA RUFA ARCOIRIS FLAVATRA</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr"/>
       <c r="D59" s="3" t="inlineStr"/>
       <c r="E59" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F59" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G59" s="4" t="n">
@@ -17398,7 +17398,7 @@
         <v>0</v>
       </c>
       <c r="L59" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M59" s="5" t="n">
         <v>0</v>
@@ -17407,7 +17407,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P59" s="4" t="n">
         <v>59</v>
@@ -17428,7 +17428,7 @@
       </c>
       <c r="U59" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 31.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.56€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V59" s="4" t="inlineStr">
@@ -17445,28 +17445,28 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>2104080001</t>
+          <t>2707130084</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>PERIQUITO BURQUE</t>
+          <t>PANCHAX RAYADO</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr"/>
       <c r="D60" s="3" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F60" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G60" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H60" s="4" t="n">
         <v>0</v>
@@ -17481,7 +17481,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M60" s="5" t="n">
         <v>0</v>
@@ -17490,19 +17490,19 @@
         <v>0</v>
       </c>
       <c r="O60" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P60" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q60" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R60" s="4" t="n">
-        <v>196.67</v>
+        <v>33.33</v>
       </c>
       <c r="S60" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T60" s="7" t="inlineStr">
         <is>
@@ -17511,12 +17511,12 @@
       </c>
       <c r="U60" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 24.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V60" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W60" s="4" t="inlineStr">
@@ -17528,12 +17528,12 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>2707080006</t>
+          <t>2707100024</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>ESCALAR RED DEVIL</t>
+          <t>APISTOGRAMA BORELLI</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr"/>
@@ -17564,7 +17564,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M61" s="5" t="n">
         <v>0</v>
@@ -17573,19 +17573,19 @@
         <v>0</v>
       </c>
       <c r="O61" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P61" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q61" s="4" t="n">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="R61" s="4" t="n">
-        <v>33.33</v>
+        <v>313.33</v>
       </c>
       <c r="S61" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T61" s="7" t="inlineStr">
         <is>
@@ -17594,12 +17594,12 @@
       </c>
       <c r="U61" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V61" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W61" s="4" t="inlineStr">
@@ -17611,24 +17611,24 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>2705040009</t>
+          <t>2707120001</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>HELECHO EN COCO PEQUEÑO</t>
+          <t>HYPANCISTRUS SP L333 5-6</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr"/>
       <c r="D62" s="3" t="inlineStr"/>
       <c r="E62" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G62" s="4" t="n">
@@ -17647,7 +17647,7 @@
         <v>0</v>
       </c>
       <c r="L62" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M62" s="5" t="n">
         <v>0</v>
@@ -17656,7 +17656,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P62" s="4" t="n">
         <v>59</v>
@@ -17677,7 +17677,7 @@
       </c>
       <c r="U62" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.52€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.64€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V62" s="4" t="inlineStr">
@@ -17694,24 +17694,32 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>2707100038</t>
+          <t>2708010010</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI BLACK DEVIL</t>
-        </is>
-      </c>
-      <c r="C63" s="3" t="inlineStr"/>
-      <c r="D63" s="3" t="inlineStr"/>
+          <t>FANTAIL SURTIDO</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="inlineStr">
+        <is>
+          <t>5CM</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F63" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G63" s="4" t="n">
@@ -17730,7 +17738,7 @@
         <v>0</v>
       </c>
       <c r="L63" s="4" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M63" s="5" t="n">
         <v>0</v>
@@ -17739,19 +17747,19 @@
         <v>0</v>
       </c>
       <c r="O63" s="4" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="P63" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q63" s="4" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="R63" s="4" t="n">
-        <v>393.33</v>
+        <v>53.33</v>
       </c>
       <c r="S63" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T63" s="7" t="inlineStr">
         <is>
@@ -17760,12 +17768,12 @@
       </c>
       <c r="U63" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 28.48€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V63" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 20/02/2025</t>
         </is>
       </c>
       <c r="W63" s="4" t="inlineStr">
@@ -17777,24 +17785,24 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>2707130054</t>
+          <t>2806030007</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>PEZ CUCHILLO PAYASO</t>
+          <t>SHUBUNKIN</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr"/>
       <c r="D64" s="3" t="inlineStr"/>
       <c r="E64" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F64" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G64" s="4" t="n">
@@ -17813,7 +17821,7 @@
         <v>0</v>
       </c>
       <c r="L64" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M64" s="5" t="n">
         <v>0</v>
@@ -17822,7 +17830,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P64" s="4" t="n">
         <v>59</v>
@@ -17843,7 +17851,7 @@
       </c>
       <c r="U64" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.09€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V64" s="4" t="inlineStr">
@@ -17860,24 +17868,24 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>2707170002</t>
+          <t>2705040008</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>PEZ SIERRA SELECTO</t>
+          <t>ANUBIA EN ROCA</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr"/>
       <c r="D65" s="3" t="inlineStr"/>
       <c r="E65" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F65" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G65" s="4" t="n">
@@ -17896,7 +17904,7 @@
         <v>0</v>
       </c>
       <c r="L65" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M65" s="5" t="n">
         <v>0</v>
@@ -17905,7 +17913,7 @@
         <v>0</v>
       </c>
       <c r="O65" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P65" s="4" t="n">
         <v>59</v>
@@ -17926,7 +17934,7 @@
       </c>
       <c r="U65" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.15€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.27€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V65" s="4" t="inlineStr">
@@ -17943,12 +17951,12 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>2707090009</t>
+          <t>2707050022</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>AULONOCARA CALICO RED NEON</t>
+          <t>BETTA KOI</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr"/>
@@ -17979,7 +17987,7 @@
         <v>0</v>
       </c>
       <c r="L66" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M66" s="5" t="n">
         <v>0</v>
@@ -17988,19 +17996,19 @@
         <v>0</v>
       </c>
       <c r="O66" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P66" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q66" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R66" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S66" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T66" s="7" t="inlineStr">
         <is>
@@ -18009,12 +18017,12 @@
       </c>
       <c r="U66" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V66" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W66" s="4" t="inlineStr">
@@ -18026,12 +18034,12 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>2707130041</t>
+          <t>2707090010</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>POPONDETA FURCATA</t>
+          <t>KANDANGO ROJO</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr"/>
@@ -18062,7 +18070,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M67" s="5" t="n">
         <v>0</v>
@@ -18071,7 +18079,7 @@
         <v>0</v>
       </c>
       <c r="O67" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P67" s="4" t="n">
         <v>59</v>
@@ -18092,7 +18100,7 @@
       </c>
       <c r="U67" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.29€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V67" s="4" t="inlineStr">
@@ -18109,24 +18117,32 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>2707070003</t>
+          <t>2705040004</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>TETRA PRISTELLA ROJA INIRIDA</t>
-        </is>
-      </c>
-      <c r="C68" s="3" t="inlineStr"/>
-      <c r="D68" s="3" t="inlineStr"/>
+          <t>PLANTAS EN TRONCO</t>
+        </is>
+      </c>
+      <c r="C68" s="3" t="inlineStr">
+        <is>
+          <t>3UD</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E68" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F68" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G68" s="4" t="n">
@@ -18145,7 +18161,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="4" t="n">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="M68" s="5" t="n">
         <v>0</v>
@@ -18154,7 +18170,7 @@
         <v>0</v>
       </c>
       <c r="O68" s="4" t="n">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="P68" s="4" t="n">
         <v>59</v>
@@ -18175,7 +18191,7 @@
       </c>
       <c r="U68" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 44.1€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 12.35€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V68" s="4" t="inlineStr">
@@ -18192,24 +18208,16 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>2707130025</t>
+          <t>2707130026</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>PANGASIUS ALBINO</t>
-        </is>
-      </c>
-      <c r="C69" s="3" t="inlineStr">
-        <is>
-          <t>6I7</t>
-        </is>
-      </c>
-      <c r="D69" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>PANGASIUS SUTCHI</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr"/>
+      <c r="D69" s="3" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -18236,7 +18244,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M69" s="5" t="n">
         <v>0</v>
@@ -18245,7 +18253,7 @@
         <v>0</v>
       </c>
       <c r="O69" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P69" s="4" t="n">
         <v>59</v>
@@ -18266,7 +18274,7 @@
       </c>
       <c r="U69" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.1€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.15€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V69" s="4" t="inlineStr">
@@ -18283,12 +18291,12 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>2707130020</t>
+          <t>2707130031</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>LABEO ZORRO VOLADOR</t>
+          <t>PEZ DOLAR PLATA</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr"/>
@@ -18319,7 +18327,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="M70" s="5" t="n">
         <v>0</v>
@@ -18328,7 +18336,7 @@
         <v>0</v>
       </c>
       <c r="O70" s="4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="P70" s="4" t="n">
         <v>59</v>
@@ -18349,7 +18357,7 @@
       </c>
       <c r="U70" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 8.32€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.35€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V70" s="4" t="inlineStr">
@@ -18366,28 +18374,28 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>2708010007</t>
+          <t>2805040003</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>COMETA SARASA</t>
+          <t>PLANTA FLOTANTE MINI</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr"/>
       <c r="D71" s="3" t="inlineStr"/>
       <c r="E71" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="F71" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PLANTAS JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G71" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H71" s="4" t="n">
         <v>0</v>
@@ -18402,7 +18410,7 @@
         <v>0</v>
       </c>
       <c r="L71" s="4" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="M71" s="5" t="n">
         <v>0</v>
@@ -18411,16 +18419,16 @@
         <v>0</v>
       </c>
       <c r="O71" s="4" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="P71" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q71" s="4" t="n">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="R71" s="4" t="n">
-        <v>393.33</v>
+        <v>173.33</v>
       </c>
       <c r="S71" s="5" t="n">
         <v>30</v>
@@ -18432,12 +18440,12 @@
       </c>
       <c r="U71" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.84€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V71" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 07/01/2025</t>
         </is>
       </c>
       <c r="W71" s="4" t="inlineStr">
@@ -18449,28 +18457,28 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>2104080003</t>
+          <t>2707050028</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>PERIQUITO INGLES (MELOPSITTACUS UNDULATUS)</t>
+          <t>BETTA HELLBOY MACHO</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr"/>
       <c r="D72" s="3" t="inlineStr"/>
       <c r="E72" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F72" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G72" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H72" s="4" t="n">
         <v>0</v>
@@ -18485,7 +18493,7 @@
         <v>0</v>
       </c>
       <c r="L72" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M72" s="5" t="n">
         <v>0</v>
@@ -18494,19 +18502,19 @@
         <v>0</v>
       </c>
       <c r="O72" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P72" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q72" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R72" s="4" t="n">
-        <v>196.67</v>
+        <v>33.33</v>
       </c>
       <c r="S72" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T72" s="7" t="inlineStr">
         <is>
@@ -18515,12 +18523,12 @@
       </c>
       <c r="U72" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 67.2€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V72" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W72" s="4" t="inlineStr">
@@ -18532,12 +18540,12 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>2606050000</t>
+          <t>2606010004</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>BICHO PALO</t>
+          <t>TORTUGA RUSA (AGRIONEMYS HORSFIELDII)</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr"/>
@@ -18568,7 +18576,7 @@
         <v>0</v>
       </c>
       <c r="L73" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M73" s="5" t="n">
         <v>0</v>
@@ -18577,19 +18585,19 @@
         <v>0</v>
       </c>
       <c r="O73" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P73" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q73" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R73" s="4" t="n">
-        <v>63.33</v>
+        <v>196.67</v>
       </c>
       <c r="S73" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T73" s="7" t="inlineStr">
         <is>
@@ -18598,12 +18606,12 @@
       </c>
       <c r="U73" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.83€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V73" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W73" s="4" t="inlineStr">
@@ -18615,24 +18623,16 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>2707110006</t>
+          <t>2707130006</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>BOTIA PAYASO</t>
-        </is>
-      </c>
-      <c r="C74" s="3" t="inlineStr">
-        <is>
-          <t>7CM</t>
-        </is>
-      </c>
-      <c r="D74" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>CRISTAL DE JAVA - BICHIRRI CRISTAL</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr"/>
+      <c r="D74" s="3" t="inlineStr"/>
       <c r="E74" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -18659,7 +18659,7 @@
         <v>0</v>
       </c>
       <c r="L74" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M74" s="5" t="n">
         <v>0</v>
@@ -18668,7 +18668,7 @@
         <v>0</v>
       </c>
       <c r="O74" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P74" s="4" t="n">
         <v>59</v>
@@ -18689,7 +18689,7 @@
       </c>
       <c r="U74" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.91€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.33€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V74" s="4" t="inlineStr">
@@ -18706,28 +18706,28 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>2606010004</t>
+          <t>2707190007</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>TORTUGA RUSA (AGRIONEMYS HORSFIELDII)</t>
+          <t>PANAQUE MAMLUS L104</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr"/>
       <c r="D75" s="3" t="inlineStr"/>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F75" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO REPTILES</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G75" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H75" s="4" t="n">
         <v>0</v>
@@ -18742,7 +18742,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M75" s="5" t="n">
         <v>0</v>
@@ -18751,7 +18751,7 @@
         <v>0</v>
       </c>
       <c r="O75" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P75" s="4" t="n">
         <v>59</v>
@@ -18760,7 +18760,7 @@
         <v>59</v>
       </c>
       <c r="R75" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S75" s="5" t="n">
         <v>30</v>
@@ -18772,7 +18772,7 @@
       </c>
       <c r="U75" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.83€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 21.39€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V75" s="4" t="inlineStr">
@@ -18789,28 +18789,28 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>2707120003</t>
+          <t>2104090006</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>LORICARIA SP RED</t>
+          <t>FORPUS MUTACION AZUL (FORPUS COELESTIS)</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr"/>
       <c r="D76" s="3" t="inlineStr"/>
       <c r="E76" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F76" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G76" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H76" s="4" t="n">
         <v>0</v>
@@ -18825,7 +18825,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M76" s="5" t="n">
         <v>0</v>
@@ -18834,7 +18834,7 @@
         <v>0</v>
       </c>
       <c r="O76" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P76" s="4" t="n">
         <v>59</v>
@@ -18843,7 +18843,7 @@
         <v>59</v>
       </c>
       <c r="R76" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S76" s="5" t="n">
         <v>30</v>
@@ -18855,7 +18855,7 @@
       </c>
       <c r="U76" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.3€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V76" s="4" t="inlineStr">
@@ -18872,12 +18872,12 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>2707170006</t>
+          <t>2707110023</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>BADIS ESCARLATA</t>
+          <t>BOTIA SUMO</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr"/>
@@ -18908,7 +18908,7 @@
         <v>0</v>
       </c>
       <c r="L77" s="4" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="M77" s="5" t="n">
         <v>0</v>
@@ -18917,7 +18917,7 @@
         <v>0</v>
       </c>
       <c r="O77" s="4" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="P77" s="4" t="n">
         <v>59</v>
@@ -18938,7 +18938,7 @@
       </c>
       <c r="U77" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.48€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V77" s="4" t="inlineStr">

</xml_diff>

<commit_message>
agrupando los archivos json
</commit_message>
<xml_diff>
--- a/data/input/CLASIFICACION_ABC+D_MASCOTAS_VIVO_P1_2025.xlsx
+++ b/data/input/CLASIFICACION_ABC+D_MASCOTAS_VIVO_P1_2025.xlsx
@@ -9009,12 +9009,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>2707130078</t>
+          <t>2707100009</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>KILLI SURTIDO</t>
+          <t>CICLIDO AMERICANO SURTIDO</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr"/>
@@ -9036,16 +9036,16 @@
         <v>4</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>29.96</v>
+        <v>25.16</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>18.04</v>
+        <v>14.07</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>8.16</v>
+        <v>200</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>0.5</v>
@@ -9054,50 +9054,50 @@
         <v>1.5</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>45</v>
+        <v>-2</v>
       </c>
       <c r="P10" s="4" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="R10" s="4" t="n">
-        <v>313.33</v>
+        <v>0</v>
       </c>
       <c r="S10" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="T10" s="7" t="inlineStr">
-        <is>
-          <t>Crítico</t>
+        <v>0</v>
+      </c>
+      <c r="T10" s="6" t="inlineStr">
+        <is>
+          <t>Bajo</t>
         </is>
       </c>
       <c r="U10" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.14€. Prioridad máxima.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -2 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
         </is>
       </c>
       <c r="V10" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Sin stock</t>
         </is>
       </c>
       <c r="W10" s="4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>25</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>2707100009</t>
+          <t>2707130078</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>CICLIDO AMERICANO SURTIDO</t>
+          <t>KILLI SURTIDO</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr"/>
@@ -9119,16 +9119,16 @@
         <v>4</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>25.16</v>
+        <v>29.96</v>
       </c>
       <c r="J11" s="4" t="n">
-        <v>14.07</v>
+        <v>18.04</v>
       </c>
       <c r="K11" s="4" t="n">
-        <v>200</v>
+        <v>8.16</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M11" s="5" t="n">
         <v>0.5</v>
@@ -9137,38 +9137,38 @@
         <v>1.5</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>-2</v>
+        <v>45</v>
       </c>
       <c r="P11" s="4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q11" s="4" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="R11" s="4" t="n">
-        <v>0</v>
+        <v>313.33</v>
       </c>
       <c r="S11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" s="6" t="inlineStr">
-        <is>
-          <t>Bajo</t>
+        <v>30</v>
+      </c>
+      <c r="T11" s="7" t="inlineStr">
+        <is>
+          <t>Crítico</t>
         </is>
       </c>
       <c r="U11" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -2 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.14€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V11" s="4" t="inlineStr">
         <is>
-          <t>Sin stock</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W11" s="4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>14</t>
         </is>
       </c>
     </row>
@@ -12599,24 +12599,24 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2104090002</t>
+          <t>2606010004</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>DIAMANTE BICHENOW (POEPHILA BICHENOVII) DIABI</t>
+          <t>TORTUGA RUSA (AGRIONEMYS HORSFIELDII)</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2606</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>ANIMAL VIVO REPTILES</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
@@ -12665,7 +12665,7 @@
       </c>
       <c r="U2" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.83€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V2" s="4" t="inlineStr">
@@ -12682,24 +12682,24 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>2708010019</t>
+          <t>2707090010</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>CABEZA DE LEON</t>
+          <t>KANDANGO ROJO</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G3" s="4" t="n">
@@ -12733,13 +12733,13 @@
         <v>59</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R3" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S3" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T3" s="7" t="inlineStr">
         <is>
@@ -12748,12 +12748,12 @@
       </c>
       <c r="U3" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.29€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V3" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W3" s="4" t="inlineStr">
@@ -12765,12 +12765,12 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>2707130035</t>
+          <t>2707130079</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>PEZ HACHA</t>
+          <t>GOBIO PAVO REAL</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr"/>
@@ -12801,7 +12801,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>0</v>
@@ -12810,7 +12810,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P4" s="4" t="n">
         <v>59</v>
@@ -12831,7 +12831,7 @@
       </c>
       <c r="U4" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.18€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.97€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V4" s="4" t="inlineStr">
@@ -12848,12 +12848,12 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>2707050019</t>
+          <t>2707100029</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>PEZ PARAISO MACROPODUS</t>
+          <t>RAMIREZI GOLD</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr"/>
@@ -12884,7 +12884,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>0</v>
@@ -12893,7 +12893,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P5" s="4" t="n">
         <v>59</v>
@@ -12914,7 +12914,7 @@
       </c>
       <c r="U5" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.96€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.59€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V5" s="4" t="inlineStr">
@@ -12931,24 +12931,24 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>2705040011</t>
+          <t>2707090009</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>BAMBU CUEVA</t>
+          <t>AULONOCARA CALICO RED NEON</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr"/>
       <c r="D6" s="3" t="inlineStr"/>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G6" s="4" t="n">
@@ -12967,7 +12967,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>0</v>
@@ -12976,7 +12976,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6" s="4" t="n">
         <v>59</v>
@@ -12997,7 +12997,7 @@
       </c>
       <c r="U6" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.32€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V6" s="4" t="inlineStr">
@@ -13014,28 +13014,28 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>2606010004</t>
+          <t>2707100028</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>TORTUGA RUSA (AGRIONEMYS HORSFIELDII)</t>
+          <t>PARACHROMIS MOTAGUENSIS 8-11 (CICLIDO JAGUAR ROJO)</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr"/>
       <c r="D7" s="3" t="inlineStr"/>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO REPTILES</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G7" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H7" s="4" t="n">
         <v>0</v>
@@ -13068,7 +13068,7 @@
         <v>59</v>
       </c>
       <c r="R7" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S7" s="5" t="n">
         <v>30</v>
@@ -13080,7 +13080,7 @@
       </c>
       <c r="U7" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.83€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.57€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V7" s="4" t="inlineStr">
@@ -13097,24 +13097,24 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>2705040009</t>
+          <t>2806030007</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>HELECHO EN COCO PEQUEÑO</t>
+          <t>SHUBUNKIN</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
       <c r="D8" s="3" t="inlineStr"/>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G8" s="4" t="n">
@@ -13133,7 +13133,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M8" s="5" t="n">
         <v>0</v>
@@ -13142,7 +13142,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P8" s="4" t="n">
         <v>59</v>
@@ -13163,7 +13163,7 @@
       </c>
       <c r="U8" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.52€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V8" s="4" t="inlineStr">
@@ -13180,12 +13180,12 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>2707050028</t>
+          <t>2707190007</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>BETTA HELLBOY MACHO</t>
+          <t>PANAQUE MAMLUS L104</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr"/>
@@ -13216,7 +13216,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" s="5" t="n">
         <v>0</v>
@@ -13225,19 +13225,19 @@
         <v>0</v>
       </c>
       <c r="O9" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P9" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q9" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R9" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S9" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T9" s="7" t="inlineStr">
         <is>
@@ -13246,12 +13246,12 @@
       </c>
       <c r="U9" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 21.39€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V9" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W9" s="4" t="inlineStr">
@@ -13263,12 +13263,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>2707110023</t>
+          <t>2707130084</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>BOTIA SUMO</t>
+          <t>PANCHAX RAYADO</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr"/>
@@ -13299,7 +13299,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>0</v>
@@ -13308,19 +13308,19 @@
         <v>0</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P10" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R10" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S10" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T10" s="7" t="inlineStr">
         <is>
@@ -13329,12 +13329,12 @@
       </c>
       <c r="U10" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V10" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W10" s="4" t="inlineStr">
@@ -13346,32 +13346,24 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>2806030001</t>
+          <t>2707110023</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>COMETA SURTIDO XXL</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>15CM</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BOTIA SUMO</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr"/>
+      <c r="D11" s="3" t="inlineStr"/>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G11" s="4" t="n">
@@ -13390,7 +13382,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M11" s="5" t="n">
         <v>0</v>
@@ -13399,7 +13391,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P11" s="4" t="n">
         <v>59</v>
@@ -13420,7 +13412,7 @@
       </c>
       <c r="U11" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.22€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V11" s="4" t="inlineStr">
@@ -13437,12 +13429,12 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>2707120003</t>
+          <t>2707130082</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>LORICARIA SP RED</t>
+          <t>RASBORA VERDE NEON</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr"/>
@@ -13473,7 +13465,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="M12" s="5" t="n">
         <v>0</v>
@@ -13482,7 +13474,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="4" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="P12" s="4" t="n">
         <v>59</v>
@@ -13503,7 +13495,7 @@
       </c>
       <c r="U12" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.3€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.13€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V12" s="4" t="inlineStr">
@@ -13520,12 +13512,12 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>2707130047</t>
+          <t>2707100040</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>RASBORA MACULATUS</t>
+          <t>RAMIREZI BOLIVIANO (PAPILIOCHROMIS ALTISPINOSA)</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr"/>
@@ -13556,7 +13548,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="M13" s="5" t="n">
         <v>0</v>
@@ -13565,16 +13557,16 @@
         <v>0</v>
       </c>
       <c r="O13" s="4" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="P13" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q13" s="4" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="R13" s="4" t="n">
-        <v>393.33</v>
+        <v>220</v>
       </c>
       <c r="S13" s="5" t="n">
         <v>30</v>
@@ -13586,12 +13578,12 @@
       </c>
       <c r="U13" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V13" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 26/01/2025</t>
         </is>
       </c>
       <c r="W13" s="4" t="inlineStr">
@@ -13603,12 +13595,12 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>2707050021</t>
+          <t>2707130020</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>BESUCON BALON</t>
+          <t>LABEO ZORRO VOLADOR</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr"/>
@@ -13639,7 +13631,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="M14" s="5" t="n">
         <v>0</v>
@@ -13648,7 +13640,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="P14" s="4" t="n">
         <v>59</v>
@@ -13669,7 +13661,7 @@
       </c>
       <c r="U14" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.04€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 8.32€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V14" s="4" t="inlineStr">
@@ -13686,12 +13678,12 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>2707120009</t>
+          <t>2707100038</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>LORICARIA FILAMENTOSA</t>
+          <t>RAMIREZI BLACK DEVIL</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr"/>
@@ -13722,7 +13714,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>0</v>
@@ -13731,7 +13723,7 @@
         <v>0</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P15" s="4" t="n">
         <v>59</v>
@@ -13752,7 +13744,7 @@
       </c>
       <c r="U15" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 19.74€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 28.48€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V15" s="4" t="inlineStr">
@@ -13769,28 +13761,28 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>2606050000</t>
+          <t>2707120003</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>BICHO PALO</t>
+          <t>LORICARIA SP RED</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
       <c r="D16" s="3" t="inlineStr"/>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO REPTILES</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G16" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H16" s="4" t="n">
         <v>0</v>
@@ -13805,7 +13797,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M16" s="5" t="n">
         <v>0</v>
@@ -13814,19 +13806,19 @@
         <v>0</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P16" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q16" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R16" s="4" t="n">
-        <v>63.33</v>
+        <v>393.33</v>
       </c>
       <c r="S16" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T16" s="7" t="inlineStr">
         <is>
@@ -13835,12 +13827,12 @@
       </c>
       <c r="U16" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.3€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V16" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W16" s="4" t="inlineStr">
@@ -13852,24 +13844,16 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>2707130025</t>
+          <t>2707110005</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>PANGASIUS ALBINO</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>6I7</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BOTIA MORLETI 4</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr"/>
+      <c r="D17" s="3" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -13896,7 +13880,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" s="5" t="n">
         <v>0</v>
@@ -13905,7 +13889,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P17" s="4" t="n">
         <v>59</v>
@@ -13926,7 +13910,7 @@
       </c>
       <c r="U17" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.1€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V17" s="4" t="inlineStr">
@@ -13943,24 +13927,32 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>2707170006</t>
+          <t>2705040004</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>BADIS ESCARLATA</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="inlineStr"/>
-      <c r="D18" s="3" t="inlineStr"/>
+          <t>PLANTAS EN TRONCO</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>3UD</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E18" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G18" s="4" t="n">
@@ -13979,7 +13971,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="M18" s="5" t="n">
         <v>0</v>
@@ -13988,7 +13980,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="P18" s="4" t="n">
         <v>59</v>
@@ -14009,7 +14001,7 @@
       </c>
       <c r="U18" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.48€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 12.35€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V18" s="4" t="inlineStr">
@@ -14026,28 +14018,28 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>2104090001</t>
+          <t>2707120009</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>DIAMANTE BARBERO COLA LARGA</t>
+          <t>LORICARIA FILAMENTOSA</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr"/>
       <c r="D19" s="3" t="inlineStr"/>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F19" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G19" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H19" s="4" t="n">
         <v>0</v>
@@ -14062,7 +14054,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M19" s="5" t="n">
         <v>0</v>
@@ -14071,7 +14063,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P19" s="4" t="n">
         <v>59</v>
@@ -14080,7 +14072,7 @@
         <v>59</v>
       </c>
       <c r="R19" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S19" s="5" t="n">
         <v>30</v>
@@ -14092,7 +14084,7 @@
       </c>
       <c r="U19" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 19.74€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V19" s="4" t="inlineStr">
@@ -14109,12 +14101,12 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>2707130021</t>
+          <t>2707120007</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>MELANOTAENIA SURTIDO</t>
+          <t>PANAQUE REAL L190</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr"/>
@@ -14145,7 +14137,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M20" s="5" t="n">
         <v>0</v>
@@ -14154,19 +14146,19 @@
         <v>0</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P20" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q20" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R20" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S20" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T20" s="7" t="inlineStr">
         <is>
@@ -14175,12 +14167,12 @@
       </c>
       <c r="U20" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.72€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V20" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W20" s="4" t="inlineStr">
@@ -14192,24 +14184,24 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>2806030007</t>
+          <t>2707130075</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>SHUBUNKIN</t>
+          <t>PEZ MEDIO PICO BUFON (HEMIRHAMPHODON KUEKENTHALI)</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr"/>
       <c r="D21" s="3" t="inlineStr"/>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G21" s="4" t="n">
@@ -14228,7 +14220,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M21" s="5" t="n">
         <v>0</v>
@@ -14237,7 +14229,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P21" s="4" t="n">
         <v>59</v>
@@ -14258,7 +14250,7 @@
       </c>
       <c r="U21" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 11.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.26€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V21" s="4" t="inlineStr">
@@ -14275,32 +14267,24 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>2708010014</t>
+          <t>2707050001</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>RYUKIN SURTIDO</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>5I6</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BESUCON HELOSTOMA TEMMINCKII</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr"/>
+      <c r="D22" s="3" t="inlineStr"/>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G22" s="4" t="n">
@@ -14319,7 +14303,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M22" s="5" t="n">
         <v>0</v>
@@ -14328,19 +14312,19 @@
         <v>0</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P22" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q22" s="4" t="n">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="R22" s="4" t="n">
-        <v>380</v>
+        <v>33.33</v>
       </c>
       <c r="S22" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T22" s="7" t="inlineStr">
         <is>
@@ -14349,12 +14333,12 @@
       </c>
       <c r="U22" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V22" s="4" t="inlineStr">
         <is>
-          <t>Compra 02/01/2025</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W22" s="4" t="inlineStr">
@@ -14366,12 +14350,12 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>2707130018</t>
+          <t>2707130035</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>GARRA RUFA ARCOIRIS FLAVATRA</t>
+          <t>PEZ HACHA</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr"/>
@@ -14402,7 +14386,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M23" s="5" t="n">
         <v>0</v>
@@ -14411,7 +14395,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P23" s="4" t="n">
         <v>59</v>
@@ -14432,7 +14416,7 @@
       </c>
       <c r="U23" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.56€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.18€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V23" s="4" t="inlineStr">
@@ -14449,16 +14433,24 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>2707050026</t>
+          <t>2707130025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>BETTA MACHO LONG TAIL</t>
-        </is>
-      </c>
-      <c r="C24" s="3" t="inlineStr"/>
-      <c r="D24" s="3" t="inlineStr"/>
+          <t>PANGASIUS ALBINO</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>6I7</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -14485,7 +14477,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M24" s="5" t="n">
         <v>0</v>
@@ -14494,7 +14486,7 @@
         <v>0</v>
       </c>
       <c r="O24" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P24" s="4" t="n">
         <v>59</v>
@@ -14515,7 +14507,7 @@
       </c>
       <c r="U24" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.92€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.1€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V24" s="4" t="inlineStr">
@@ -14532,28 +14524,28 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>2705040010</t>
+          <t>2606050000</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>BAMBU PIRAMIDE</t>
+          <t>BICHO PALO</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr"/>
       <c r="D25" s="3" t="inlineStr"/>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2606</t>
         </is>
       </c>
       <c r="F25" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>ANIMAL VIVO REPTILES</t>
         </is>
       </c>
       <c r="G25" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H25" s="4" t="n">
         <v>0</v>
@@ -14568,7 +14560,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M25" s="5" t="n">
         <v>0</v>
@@ -14577,19 +14569,19 @@
         <v>0</v>
       </c>
       <c r="O25" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P25" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q25" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R25" s="4" t="n">
-        <v>393.33</v>
+        <v>63.33</v>
       </c>
       <c r="S25" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T25" s="7" t="inlineStr">
         <is>
@@ -14598,12 +14590,12 @@
       </c>
       <c r="U25" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.98€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V25" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W25" s="4" t="inlineStr">
@@ -14615,24 +14607,24 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>2707090009</t>
+          <t>2708010014</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>AULONOCARA CALICO RED NEON</t>
+          <t>RYUKIN SURTIDO</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr"/>
       <c r="D26" s="3" t="inlineStr"/>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F26" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G26" s="4" t="n">
@@ -14651,7 +14643,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M26" s="5" t="n">
         <v>0</v>
@@ -14660,7 +14652,7 @@
         <v>0</v>
       </c>
       <c r="O26" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P26" s="4" t="n">
         <v>59</v>
@@ -14681,7 +14673,7 @@
       </c>
       <c r="U26" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 31.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V26" s="4" t="inlineStr">
@@ -14698,24 +14690,24 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>2707130020</t>
+          <t>2705040003</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>LABEO ZORRO VOLADOR</t>
+          <t>PLANTA ACUATICA XL</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr"/>
       <c r="D27" s="3" t="inlineStr"/>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F27" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G27" s="4" t="n">
@@ -14734,7 +14726,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="M27" s="5" t="n">
         <v>0</v>
@@ -14743,7 +14735,7 @@
         <v>0</v>
       </c>
       <c r="O27" s="4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="P27" s="4" t="n">
         <v>59</v>
@@ -14764,7 +14756,7 @@
       </c>
       <c r="U27" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 8.32€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.29€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V27" s="4" t="inlineStr">
@@ -14781,12 +14773,12 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>2707040006</t>
+          <t>2707130083</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>BARBO ARCOIRIS (NOTROPIS CHROSOMUS)</t>
+          <t>POPONDETA PASKAI</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr"/>
@@ -14817,7 +14809,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="4" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="M28" s="5" t="n">
         <v>0</v>
@@ -14826,19 +14818,19 @@
         <v>0</v>
       </c>
       <c r="O28" s="4" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="P28" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q28" s="4" t="n">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="R28" s="4" t="n">
-        <v>33.33</v>
+        <v>313.33</v>
       </c>
       <c r="S28" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T28" s="7" t="inlineStr">
         <is>
@@ -14847,12 +14839,12 @@
       </c>
       <c r="U28" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V28" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W28" s="4" t="inlineStr">
@@ -14864,28 +14856,28 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>2707130075</t>
+          <t>2104080003</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>PEZ MEDIO PICO BUFON (HEMIRHAMPHODON KUEKENTHALI)</t>
+          <t>PERIQUITO INGLES (MELOPSITTACUS UNDULATUS)</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr"/>
       <c r="D29" s="3" t="inlineStr"/>
       <c r="E29" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F29" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G29" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H29" s="4" t="n">
         <v>0</v>
@@ -14918,7 +14910,7 @@
         <v>59</v>
       </c>
       <c r="R29" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S29" s="5" t="n">
         <v>30</v>
@@ -14930,7 +14922,7 @@
       </c>
       <c r="U29" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.26€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 67.2€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V29" s="4" t="inlineStr">
@@ -14947,12 +14939,12 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>2707130083</t>
+          <t>2707130006</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>POPONDETA PASKAI</t>
+          <t>CRISTAL DE JAVA - BICHIRRI CRISTAL</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr"/>
@@ -14983,7 +14975,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M30" s="5" t="n">
         <v>0</v>
@@ -14992,16 +14984,16 @@
         <v>0</v>
       </c>
       <c r="O30" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P30" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q30" s="4" t="n">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="R30" s="4" t="n">
-        <v>313.33</v>
+        <v>393.33</v>
       </c>
       <c r="S30" s="5" t="n">
         <v>30</v>
@@ -15013,12 +15005,12 @@
       </c>
       <c r="U30" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.33€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V30" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W30" s="4" t="inlineStr">
@@ -15030,12 +15022,12 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>2707130041</t>
+          <t>2707130021</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>POPONDETA FURCATA</t>
+          <t>MELANOTAENIA SURTIDO</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr"/>
@@ -15066,7 +15058,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M31" s="5" t="n">
         <v>0</v>
@@ -15075,19 +15067,19 @@
         <v>0</v>
       </c>
       <c r="O31" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P31" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q31" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R31" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S31" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T31" s="7" t="inlineStr">
         <is>
@@ -15096,12 +15088,12 @@
       </c>
       <c r="U31" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V31" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W31" s="4" t="inlineStr">
@@ -15113,12 +15105,12 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>2707130054</t>
+          <t>2707050021</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>PEZ CUCHILLO PAYASO</t>
+          <t>BESUCON BALON</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr"/>
@@ -15149,7 +15141,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M32" s="5" t="n">
         <v>0</v>
@@ -15158,7 +15150,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P32" s="4" t="n">
         <v>59</v>
@@ -15179,7 +15171,7 @@
       </c>
       <c r="U32" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.09€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.04€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V32" s="4" t="inlineStr">
@@ -15196,12 +15188,12 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>2707050001</t>
+          <t>2707130026</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>BESUCON HELOSTOMA TEMMINCKII</t>
+          <t>PANGASIUS SUTCHI</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr"/>
@@ -15232,7 +15224,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M33" s="5" t="n">
         <v>0</v>
@@ -15241,19 +15233,19 @@
         <v>0</v>
       </c>
       <c r="O33" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P33" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q33" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R33" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S33" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T33" s="7" t="inlineStr">
         <is>
@@ -15262,12 +15254,12 @@
       </c>
       <c r="U33" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.15€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V33" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W33" s="4" t="inlineStr">
@@ -15279,24 +15271,24 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>2708010014</t>
+          <t>2707130054</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>RYUKIN SURTIDO</t>
+          <t>PEZ CUCHILLO PAYASO</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr"/>
       <c r="D34" s="3" t="inlineStr"/>
       <c r="E34" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F34" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G34" s="4" t="n">
@@ -15315,7 +15307,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M34" s="5" t="n">
         <v>0</v>
@@ -15324,7 +15316,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P34" s="4" t="n">
         <v>59</v>
@@ -15345,7 +15337,7 @@
       </c>
       <c r="U34" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 31.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.09€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V34" s="4" t="inlineStr">
@@ -15362,12 +15354,12 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>2707100016</t>
+          <t>2707120001</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI ALEMAN AZUL (MIKROGEOPHAGUS)</t>
+          <t>HYPANCISTRUS SP L333 5-6</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr"/>
@@ -15398,7 +15390,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M35" s="5" t="n">
         <v>0</v>
@@ -15407,16 +15399,16 @@
         <v>0</v>
       </c>
       <c r="O35" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P35" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q35" s="4" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="R35" s="4" t="n">
-        <v>220</v>
+        <v>393.33</v>
       </c>
       <c r="S35" s="5" t="n">
         <v>30</v>
@@ -15428,12 +15420,12 @@
       </c>
       <c r="U35" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.64€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V35" s="4" t="inlineStr">
         <is>
-          <t>Compra 26/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W35" s="4" t="inlineStr">
@@ -15445,28 +15437,28 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>2104090006</t>
+          <t>2705040010</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>FORPUS MUTACION AZUL (FORPUS COELESTIS)</t>
+          <t>BAMBU PIRAMIDE</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr"/>
       <c r="D36" s="3" t="inlineStr"/>
       <c r="E36" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F36" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G36" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H36" s="4" t="n">
         <v>0</v>
@@ -15481,7 +15473,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M36" s="5" t="n">
         <v>0</v>
@@ -15490,7 +15482,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P36" s="4" t="n">
         <v>59</v>
@@ -15499,7 +15491,7 @@
         <v>59</v>
       </c>
       <c r="R36" s="4" t="n">
-        <v>196.67</v>
+        <v>393.33</v>
       </c>
       <c r="S36" s="5" t="n">
         <v>30</v>
@@ -15511,7 +15503,7 @@
       </c>
       <c r="U36" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.98€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V36" s="4" t="inlineStr">
@@ -15528,24 +15520,16 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>2707110006</t>
+          <t>2707100011</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>BOTIA PAYASO</t>
-        </is>
-      </c>
-      <c r="C37" s="3" t="inlineStr">
-        <is>
-          <t>7CM</t>
-        </is>
-      </c>
-      <c r="D37" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>HEROS SEVERUM</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr"/>
+      <c r="D37" s="3" t="inlineStr"/>
       <c r="E37" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -15587,10 +15571,10 @@
         <v>59</v>
       </c>
       <c r="Q37" s="4" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="R37" s="4" t="n">
-        <v>393.33</v>
+        <v>313.33</v>
       </c>
       <c r="S37" s="5" t="n">
         <v>30</v>
@@ -15602,12 +15586,12 @@
       </c>
       <c r="U37" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.91€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V37" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W37" s="4" t="inlineStr">
@@ -15619,28 +15603,28 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>2707100011</t>
+          <t>2104090002</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>HEROS SEVERUM</t>
+          <t>DIAMANTE BICHENOW (POEPHILA BICHENOVII) DIABI</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr"/>
       <c r="D38" s="3" t="inlineStr"/>
       <c r="E38" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F38" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G38" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H38" s="4" t="n">
         <v>0</v>
@@ -15655,7 +15639,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M38" s="5" t="n">
         <v>0</v>
@@ -15664,16 +15648,16 @@
         <v>0</v>
       </c>
       <c r="O38" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P38" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q38" s="4" t="n">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="R38" s="4" t="n">
-        <v>313.33</v>
+        <v>196.67</v>
       </c>
       <c r="S38" s="5" t="n">
         <v>30</v>
@@ -15685,12 +15669,12 @@
       </c>
       <c r="U38" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V38" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W38" s="4" t="inlineStr">
@@ -15702,12 +15686,12 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>2707100029</t>
+          <t>2707100013</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI GOLD</t>
+          <t>NANACARA ANOMALA</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr"/>
@@ -15738,7 +15722,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M39" s="5" t="n">
         <v>0</v>
@@ -15747,19 +15731,19 @@
         <v>0</v>
       </c>
       <c r="O39" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P39" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q39" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R39" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S39" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T39" s="7" t="inlineStr">
         <is>
@@ -15768,12 +15752,12 @@
       </c>
       <c r="U39" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.59€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V39" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W39" s="4" t="inlineStr">
@@ -15868,12 +15852,12 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>2707110022</t>
+          <t>2707130041</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>CORYDORA ORANGE VENEZUELA</t>
+          <t>POPONDETA FURCATA</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr"/>
@@ -15904,7 +15888,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M41" s="5" t="n">
         <v>0</v>
@@ -15913,7 +15897,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P41" s="4" t="n">
         <v>59</v>
@@ -15934,7 +15918,7 @@
       </c>
       <c r="U41" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 9.58€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V41" s="4" t="inlineStr">
@@ -15951,12 +15935,12 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>2707080006</t>
+          <t>2707130018</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>ESCALAR RED DEVIL</t>
+          <t>GARRA RUFA ARCOIRIS FLAVATRA</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr"/>
@@ -15987,7 +15971,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M42" s="5" t="n">
         <v>0</v>
@@ -15996,19 +15980,19 @@
         <v>0</v>
       </c>
       <c r="O42" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P42" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q42" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R42" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S42" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T42" s="7" t="inlineStr">
         <is>
@@ -16017,12 +16001,12 @@
       </c>
       <c r="U42" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.56€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V42" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W42" s="4" t="inlineStr">
@@ -16034,12 +16018,12 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>2707100013</t>
+          <t>2707130031</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>NANACARA ANOMALA</t>
+          <t>PEZ DOLAR PLATA</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr"/>
@@ -16070,7 +16054,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M43" s="5" t="n">
         <v>0</v>
@@ -16079,19 +16063,19 @@
         <v>0</v>
       </c>
       <c r="O43" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P43" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q43" s="4" t="n">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="R43" s="4" t="n">
-        <v>126.67</v>
+        <v>393.33</v>
       </c>
       <c r="S43" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T43" s="7" t="inlineStr">
         <is>
@@ -16100,12 +16084,12 @@
       </c>
       <c r="U43" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.35€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V43" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W43" s="4" t="inlineStr">
@@ -16117,32 +16101,24 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>2708010010</t>
+          <t>2707050019</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>FANTAIL SURTIDO</t>
-        </is>
-      </c>
-      <c r="C44" s="3" t="inlineStr">
-        <is>
-          <t>5CM</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>PEZ PARAISO MACROPODUS</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr"/>
+      <c r="D44" s="3" t="inlineStr"/>
       <c r="E44" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F44" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G44" s="4" t="n">
@@ -16161,7 +16137,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="4" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M44" s="5" t="n">
         <v>0</v>
@@ -16170,19 +16146,19 @@
         <v>0</v>
       </c>
       <c r="O44" s="4" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="P44" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q44" s="4" t="n">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="R44" s="4" t="n">
-        <v>53.33</v>
+        <v>393.33</v>
       </c>
       <c r="S44" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T44" s="7" t="inlineStr">
         <is>
@@ -16191,12 +16167,12 @@
       </c>
       <c r="U44" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.96€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V44" s="4" t="inlineStr">
         <is>
-          <t>Compra 20/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W44" s="4" t="inlineStr">
@@ -16208,12 +16184,12 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>2707050022</t>
+          <t>2707100016</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>BETTA KOI</t>
+          <t>RAMIREZI ALEMAN AZUL (MIKROGEOPHAGUS)</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr"/>
@@ -16244,7 +16220,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M45" s="5" t="n">
         <v>0</v>
@@ -16253,19 +16229,19 @@
         <v>0</v>
       </c>
       <c r="O45" s="4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P45" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q45" s="4" t="n">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="R45" s="4" t="n">
-        <v>126.67</v>
+        <v>220</v>
       </c>
       <c r="S45" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="T45" s="7" t="inlineStr">
         <is>
@@ -16274,12 +16250,12 @@
       </c>
       <c r="U45" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V45" s="4" t="inlineStr">
         <is>
-          <t>Compra 09/02/2025</t>
+          <t>Compra 26/01/2025</t>
         </is>
       </c>
       <c r="W45" s="4" t="inlineStr">
@@ -16291,12 +16267,12 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>2707170002</t>
+          <t>2707080006</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>PEZ SIERRA SELECTO</t>
+          <t>ESCALAR RED DEVIL</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr"/>
@@ -16327,7 +16303,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M46" s="5" t="n">
         <v>0</v>
@@ -16336,19 +16312,19 @@
         <v>0</v>
       </c>
       <c r="O46" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P46" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q46" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R46" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S46" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T46" s="7" t="inlineStr">
         <is>
@@ -16357,12 +16333,12 @@
       </c>
       <c r="U46" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.15€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V46" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W46" s="4" t="inlineStr">
@@ -16374,28 +16350,36 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>2805040003</t>
+          <t>2708010014</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>PLANTA FLOTANTE MINI</t>
-        </is>
-      </c>
-      <c r="C47" s="3" t="inlineStr"/>
-      <c r="D47" s="3" t="inlineStr"/>
+          <t>RYUKIN SURTIDO</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>5I6</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F47" s="4" t="inlineStr">
         <is>
-          <t>PLANTAS JARDIN ACUATICO</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G47" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H47" s="4" t="n">
         <v>0</v>
@@ -16410,7 +16394,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="4" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="M47" s="5" t="n">
         <v>0</v>
@@ -16419,16 +16403,16 @@
         <v>0</v>
       </c>
       <c r="O47" s="4" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="P47" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q47" s="4" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R47" s="4" t="n">
-        <v>173.33</v>
+        <v>380</v>
       </c>
       <c r="S47" s="5" t="n">
         <v>30</v>
@@ -16445,7 +16429,7 @@
       </c>
       <c r="V47" s="4" t="inlineStr">
         <is>
-          <t>Compra 07/01/2025</t>
+          <t>Compra 02/01/2025</t>
         </is>
       </c>
       <c r="W47" s="4" t="inlineStr">
@@ -16457,12 +16441,12 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>2104080001</t>
+          <t>2104090006</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>PERIQUITO BURQUE</t>
+          <t>FORPUS MUTACION AZUL (FORPUS COELESTIS)</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr"/>
@@ -16493,7 +16477,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M48" s="5" t="n">
         <v>0</v>
@@ -16502,7 +16486,7 @@
         <v>0</v>
       </c>
       <c r="O48" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P48" s="4" t="n">
         <v>59</v>
@@ -16523,7 +16507,7 @@
       </c>
       <c r="U48" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 24.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 49.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V48" s="4" t="inlineStr">
@@ -16540,12 +16524,12 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>2707130026</t>
+          <t>2707170002</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>PANGASIUS SUTCHI</t>
+          <t>PEZ SIERRA SELECTO</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr"/>
@@ -16576,7 +16560,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M49" s="5" t="n">
         <v>0</v>
@@ -16585,7 +16569,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P49" s="4" t="n">
         <v>59</v>
@@ -16606,7 +16590,7 @@
       </c>
       <c r="U49" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.15€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.15€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V49" s="4" t="inlineStr">
@@ -16623,16 +16607,24 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>2707130079</t>
+          <t>2707110006</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>GOBIO PAVO REAL</t>
-        </is>
-      </c>
-      <c r="C50" s="3" t="inlineStr"/>
-      <c r="D50" s="3" t="inlineStr"/>
+          <t>BOTIA PAYASO</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>7CM</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E50" s="4" t="inlineStr">
         <is>
           <t>2707</t>
@@ -16659,7 +16651,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M50" s="5" t="n">
         <v>0</v>
@@ -16668,7 +16660,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P50" s="4" t="n">
         <v>59</v>
@@ -16689,7 +16681,7 @@
       </c>
       <c r="U50" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 4.97€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.91€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V50" s="4" t="inlineStr">
@@ -16706,12 +16698,12 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>2707090010</t>
+          <t>2707040007</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>KANDANGO ROJO</t>
+          <t>BARBO SAWBWA</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr"/>
@@ -16742,7 +16734,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M51" s="5" t="n">
         <v>0</v>
@@ -16751,19 +16743,19 @@
         <v>0</v>
       </c>
       <c r="O51" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P51" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q51" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R51" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S51" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T51" s="7" t="inlineStr">
         <is>
@@ -16772,12 +16764,12 @@
       </c>
       <c r="U51" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.29€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V51" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W51" s="4" t="inlineStr">
@@ -16789,28 +16781,28 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>2707130006</t>
+          <t>2805040003</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>CRISTAL DE JAVA - BICHIRRI CRISTAL</t>
+          <t>PLANTA FLOTANTE MINI</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr"/>
       <c r="D52" s="3" t="inlineStr"/>
       <c r="E52" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="F52" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTAS JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G52" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H52" s="4" t="n">
         <v>0</v>
@@ -16825,7 +16817,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="4" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="M52" s="5" t="n">
         <v>0</v>
@@ -16834,16 +16826,16 @@
         <v>0</v>
       </c>
       <c r="O52" s="4" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="P52" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q52" s="4" t="n">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="R52" s="4" t="n">
-        <v>393.33</v>
+        <v>173.33</v>
       </c>
       <c r="S52" s="5" t="n">
         <v>30</v>
@@ -16855,12 +16847,12 @@
       </c>
       <c r="U52" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.33€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V52" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 07/01/2025</t>
         </is>
       </c>
       <c r="W52" s="4" t="inlineStr">
@@ -16872,28 +16864,28 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>2104080003</t>
+          <t>2708010019</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>PERIQUITO INGLES (MELOPSITTACUS UNDULATUS)</t>
+          <t>CABEZA DE LEON</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr"/>
       <c r="D53" s="3" t="inlineStr"/>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F53" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PAJARO</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G53" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H53" s="4" t="n">
         <v>0</v>
@@ -16908,7 +16900,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M53" s="5" t="n">
         <v>0</v>
@@ -16917,19 +16909,19 @@
         <v>0</v>
       </c>
       <c r="O53" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P53" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q53" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R53" s="4" t="n">
-        <v>196.67</v>
+        <v>126.67</v>
       </c>
       <c r="S53" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T53" s="7" t="inlineStr">
         <is>
@@ -16938,12 +16930,12 @@
       </c>
       <c r="U53" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 67.2€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V53" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W53" s="4" t="inlineStr">
@@ -16955,24 +16947,24 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>2707100002</t>
+          <t>2708020003</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>ANDINOACARA PULCHER AZUL ELECTRICO 3-4</t>
+          <t>ORANDA SURTIDO</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr"/>
       <c r="D54" s="3" t="inlineStr"/>
       <c r="E54" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F54" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G54" s="4" t="n">
@@ -16991,7 +16983,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="4" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="M54" s="5" t="n">
         <v>0</v>
@@ -17000,7 +16992,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="4" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="P54" s="4" t="n">
         <v>59</v>
@@ -17021,7 +17013,7 @@
       </c>
       <c r="U54" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.47€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 59.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V54" s="4" t="inlineStr">
@@ -17038,24 +17030,24 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>2707130084</t>
+          <t>2806030001</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>PANCHAX RAYADO</t>
+          <t>COMETA SURTIDO XXL</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr"/>
       <c r="D55" s="3" t="inlineStr"/>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F55" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G55" s="4" t="n">
@@ -17074,7 +17066,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="4" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="M55" s="5" t="n">
         <v>0</v>
@@ -17083,19 +17075,19 @@
         <v>0</v>
       </c>
       <c r="O55" s="4" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="P55" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q55" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R55" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S55" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T55" s="7" t="inlineStr">
         <is>
@@ -17104,12 +17096,12 @@
       </c>
       <c r="U55" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 51.56€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V55" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W55" s="4" t="inlineStr">
@@ -17121,28 +17113,28 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>2705040008</t>
+          <t>2104090001</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>ANUBIA EN ROCA</t>
+          <t>DIAMANTE BARBERO COLA LARGA</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr"/>
       <c r="D56" s="3" t="inlineStr"/>
       <c r="E56" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F56" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G56" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H56" s="4" t="n">
         <v>0</v>
@@ -17157,7 +17149,7 @@
         <v>0</v>
       </c>
       <c r="L56" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M56" s="5" t="n">
         <v>0</v>
@@ -17166,7 +17158,7 @@
         <v>0</v>
       </c>
       <c r="O56" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P56" s="4" t="n">
         <v>59</v>
@@ -17175,7 +17167,7 @@
         <v>59</v>
       </c>
       <c r="R56" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S56" s="5" t="n">
         <v>30</v>
@@ -17187,7 +17179,7 @@
       </c>
       <c r="U56" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.27€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V56" s="4" t="inlineStr">
@@ -17287,24 +17279,32 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>2707100024</t>
+          <t>2708010010</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>APISTOGRAMA BORELLI</t>
-        </is>
-      </c>
-      <c r="C58" s="3" t="inlineStr"/>
-      <c r="D58" s="3" t="inlineStr"/>
+          <t>FANTAIL SURTIDO</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="inlineStr">
+        <is>
+          <t>5CM</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E58" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES AGUA FRIA ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G58" s="4" t="n">
@@ -17323,7 +17323,7 @@
         <v>0</v>
       </c>
       <c r="L58" s="4" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M58" s="5" t="n">
         <v>0</v>
@@ -17332,19 +17332,19 @@
         <v>0</v>
       </c>
       <c r="O58" s="4" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="P58" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q58" s="4" t="n">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="R58" s="4" t="n">
-        <v>313.33</v>
+        <v>53.33</v>
       </c>
       <c r="S58" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T58" s="7" t="inlineStr">
         <is>
@@ -17353,12 +17353,12 @@
       </c>
       <c r="U58" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V58" s="4" t="inlineStr">
         <is>
-          <t>Compra 12/01/2025</t>
+          <t>Compra 20/02/2025</t>
         </is>
       </c>
       <c r="W58" s="4" t="inlineStr">
@@ -17370,24 +17370,24 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>2707100028</t>
+          <t>2705040011</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>PARACHROMIS MOTAGUENSIS 8-11 (CICLIDO JAGUAR ROJO)</t>
+          <t>BAMBU CUEVA</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr"/>
       <c r="D59" s="3" t="inlineStr"/>
       <c r="E59" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F59" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G59" s="4" t="n">
@@ -17406,7 +17406,7 @@
         <v>0</v>
       </c>
       <c r="L59" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M59" s="5" t="n">
         <v>0</v>
@@ -17415,7 +17415,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P59" s="4" t="n">
         <v>59</v>
@@ -17436,7 +17436,7 @@
       </c>
       <c r="U59" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.57€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.32€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V59" s="4" t="inlineStr">
@@ -17453,12 +17453,12 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>2708020003</t>
+          <t>2708010007</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>ORANDA SURTIDO</t>
+          <t>COMETA SARASA</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr"/>
@@ -17489,7 +17489,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="4" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="M60" s="5" t="n">
         <v>0</v>
@@ -17498,7 +17498,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="4" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="P60" s="4" t="n">
         <v>59</v>
@@ -17519,7 +17519,7 @@
       </c>
       <c r="U60" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 59.5€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.84€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V60" s="4" t="inlineStr">
@@ -17536,12 +17536,12 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>2707120001</t>
+          <t>2707100024</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>HYPANCISTRUS SP L333 5-6</t>
+          <t>APISTOGRAMA BORELLI</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr"/>
@@ -17572,7 +17572,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M61" s="5" t="n">
         <v>0</v>
@@ -17581,16 +17581,16 @@
         <v>0</v>
       </c>
       <c r="O61" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P61" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q61" s="4" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="R61" s="4" t="n">
-        <v>393.33</v>
+        <v>313.33</v>
       </c>
       <c r="S61" s="5" t="n">
         <v>30</v>
@@ -17602,12 +17602,12 @@
       </c>
       <c r="U61" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.64€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V61" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 12/01/2025</t>
         </is>
       </c>
       <c r="W61" s="4" t="inlineStr">
@@ -17619,24 +17619,24 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>2806030001</t>
+          <t>2707050026</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>COMETA SURTIDO XXL</t>
+          <t>BETTA MACHO LONG TAIL</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr"/>
       <c r="D62" s="3" t="inlineStr"/>
       <c r="E62" s="4" t="inlineStr">
         <is>
-          <t>2806</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>PECES JARDIN ACUATICO</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G62" s="4" t="n">
@@ -17655,7 +17655,7 @@
         <v>0</v>
       </c>
       <c r="L62" s="4" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="M62" s="5" t="n">
         <v>0</v>
@@ -17664,7 +17664,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="4" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="P62" s="4" t="n">
         <v>59</v>
@@ -17685,7 +17685,7 @@
       </c>
       <c r="U62" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 51.56€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.92€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V62" s="4" t="inlineStr">
@@ -17702,24 +17702,24 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>2707100004</t>
+          <t>2705040009</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>APISTOGRAMA CACATUOIDES</t>
+          <t>HELECHO EN COCO PEQUEÑO</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr"/>
       <c r="D63" s="3" t="inlineStr"/>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F63" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G63" s="4" t="n">
@@ -17768,7 +17768,7 @@
       </c>
       <c r="U63" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.79€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 6.52€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V63" s="4" t="inlineStr">
@@ -17785,28 +17785,28 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>2708010007</t>
+          <t>2104080001</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>COMETA SARASA</t>
+          <t>PERIQUITO BURQUE</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr"/>
       <c r="D64" s="3" t="inlineStr"/>
       <c r="E64" s="4" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>2104</t>
         </is>
       </c>
       <c r="F64" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA FRIA ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PAJARO</t>
         </is>
       </c>
       <c r="G64" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H64" s="4" t="n">
         <v>0</v>
@@ -17821,7 +17821,7 @@
         <v>0</v>
       </c>
       <c r="L64" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M64" s="5" t="n">
         <v>0</v>
@@ -17830,7 +17830,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P64" s="4" t="n">
         <v>59</v>
@@ -17839,7 +17839,7 @@
         <v>59</v>
       </c>
       <c r="R64" s="4" t="n">
-        <v>393.33</v>
+        <v>196.67</v>
       </c>
       <c r="S64" s="5" t="n">
         <v>30</v>
@@ -17851,7 +17851,7 @@
       </c>
       <c r="U64" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 7.84€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 24.5€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V64" s="4" t="inlineStr">
@@ -17868,12 +17868,12 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>2707100040</t>
+          <t>2707170006</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI BOLIVIANO (PAPILIOCHROMIS ALTISPINOSA)</t>
+          <t>BADIS ESCARLATA</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr"/>
@@ -17904,7 +17904,7 @@
         <v>0</v>
       </c>
       <c r="L65" s="4" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="M65" s="5" t="n">
         <v>0</v>
@@ -17913,16 +17913,16 @@
         <v>0</v>
       </c>
       <c r="O65" s="4" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="P65" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q65" s="4" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="R65" s="4" t="n">
-        <v>220</v>
+        <v>393.33</v>
       </c>
       <c r="S65" s="5" t="n">
         <v>30</v>
@@ -17934,12 +17934,12 @@
       </c>
       <c r="U65" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 20.48€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V65" s="4" t="inlineStr">
         <is>
-          <t>Compra 26/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W65" s="4" t="inlineStr">
@@ -17951,12 +17951,12 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>2707120007</t>
+          <t>2707130047</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>PANAQUE REAL L190</t>
+          <t>RASBORA MACULATUS</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr"/>
@@ -17987,7 +17987,7 @@
         <v>0</v>
       </c>
       <c r="L66" s="4" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="M66" s="5" t="n">
         <v>0</v>
@@ -17996,7 +17996,7 @@
         <v>0</v>
       </c>
       <c r="O66" s="4" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="P66" s="4" t="n">
         <v>59</v>
@@ -18017,7 +18017,7 @@
       </c>
       <c r="U66" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.72€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 15.31€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V66" s="4" t="inlineStr">
@@ -18034,12 +18034,12 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>2707130082</t>
+          <t>2707050022</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>RASBORA VERDE NEON</t>
+          <t>BETTA KOI</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr"/>
@@ -18070,7 +18070,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="4" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="M67" s="5" t="n">
         <v>0</v>
@@ -18079,19 +18079,19 @@
         <v>0</v>
       </c>
       <c r="O67" s="4" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="P67" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q67" s="4" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="R67" s="4" t="n">
-        <v>393.33</v>
+        <v>126.67</v>
       </c>
       <c r="S67" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T67" s="7" t="inlineStr">
         <is>
@@ -18100,12 +18100,12 @@
       </c>
       <c r="U67" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 43.13€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V67" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 09/02/2025</t>
         </is>
       </c>
       <c r="W67" s="4" t="inlineStr">
@@ -18117,12 +18117,12 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>2707100038</t>
+          <t>2707050028</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>RAMIREZI BLACK DEVIL</t>
+          <t>BETTA HELLBOY MACHO</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr"/>
@@ -18153,7 +18153,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M68" s="5" t="n">
         <v>0</v>
@@ -18162,19 +18162,19 @@
         <v>0</v>
       </c>
       <c r="O68" s="4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P68" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q68" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R68" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S68" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T68" s="7" t="inlineStr">
         <is>
@@ -18183,12 +18183,12 @@
       </c>
       <c r="U68" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 28.48€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V68" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W68" s="4" t="inlineStr">
@@ -18200,12 +18200,12 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>2707130031</t>
+          <t>2707040006</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>PEZ DOLAR PLATA</t>
+          <t>BARBO ARCOIRIS (NOTROPIS CHROSOMUS)</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr"/>
@@ -18236,7 +18236,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="4" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="M69" s="5" t="n">
         <v>0</v>
@@ -18245,19 +18245,19 @@
         <v>0</v>
       </c>
       <c r="O69" s="4" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="P69" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q69" s="4" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="R69" s="4" t="n">
-        <v>393.33</v>
+        <v>33.33</v>
       </c>
       <c r="S69" s="5" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T69" s="7" t="inlineStr">
         <is>
@@ -18266,12 +18266,12 @@
       </c>
       <c r="U69" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.35€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V69" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 23/02/2025</t>
         </is>
       </c>
       <c r="W69" s="4" t="inlineStr">
@@ -18283,28 +18283,28 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>2707110001</t>
+          <t>2204010007</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>BOTIA CARA CABALLO</t>
+          <t>CONEJO SUPER TOY PEDIGRI (ORYCTOLAGUS CUNICULUS)</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr"/>
       <c r="D70" s="3" t="inlineStr"/>
       <c r="E70" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2204</t>
         </is>
       </c>
       <c r="F70" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>ANIMAL VIVO PEQUEÑOS MAMIFEROS</t>
         </is>
       </c>
       <c r="G70" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H70" s="4" t="n">
         <v>0</v>
@@ -18319,7 +18319,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M70" s="5" t="n">
         <v>0</v>
@@ -18328,16 +18328,16 @@
         <v>0</v>
       </c>
       <c r="O70" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P70" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q70" s="4" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R70" s="4" t="n">
-        <v>393.33</v>
+        <v>190</v>
       </c>
       <c r="S70" s="5" t="n">
         <v>30</v>
@@ -18349,12 +18349,12 @@
       </c>
       <c r="U70" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.54€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V70" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 02/01/2025</t>
         </is>
       </c>
       <c r="W70" s="4" t="inlineStr">
@@ -18366,12 +18366,12 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>2707070003</t>
+          <t>2707100002</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>TETRA PRISTELLA ROJA INIRIDA</t>
+          <t>ANDINOACARA PULCHER AZUL ELECTRICO 3-4</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr"/>
@@ -18402,7 +18402,7 @@
         <v>0</v>
       </c>
       <c r="L71" s="4" t="n">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="M71" s="5" t="n">
         <v>0</v>
@@ -18411,7 +18411,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="4" t="n">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="P71" s="4" t="n">
         <v>59</v>
@@ -18432,7 +18432,7 @@
       </c>
       <c r="U71" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 44.1€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 1.47€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V71" s="4" t="inlineStr">
@@ -18449,24 +18449,24 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>2707040007</t>
+          <t>2705040008</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>BARBO SAWBWA</t>
+          <t>ANUBIA EN ROCA</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr"/>
       <c r="D72" s="3" t="inlineStr"/>
       <c r="E72" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2705</t>
         </is>
       </c>
       <c r="F72" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G72" s="4" t="n">
@@ -18485,7 +18485,7 @@
         <v>0</v>
       </c>
       <c r="L72" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M72" s="5" t="n">
         <v>0</v>
@@ -18494,19 +18494,19 @@
         <v>0</v>
       </c>
       <c r="O72" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="P72" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q72" s="4" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="R72" s="4" t="n">
-        <v>33.33</v>
+        <v>393.33</v>
       </c>
       <c r="S72" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T72" s="7" t="inlineStr">
         <is>
@@ -18515,12 +18515,12 @@
       </c>
       <c r="U72" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 10.27€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V72" s="4" t="inlineStr">
         <is>
-          <t>Compra 23/02/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W72" s="4" t="inlineStr">
@@ -18532,28 +18532,28 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>2204010007</t>
+          <t>2707110001</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>CONEJO SUPER TOY PEDIGRI (ORYCTOLAGUS CUNICULUS)</t>
+          <t>BOTIA CARA CABALLO</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr"/>
       <c r="D73" s="3" t="inlineStr"/>
       <c r="E73" s="4" t="inlineStr">
         <is>
-          <t>2204</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F73" s="4" t="inlineStr">
         <is>
-          <t>ANIMAL VIVO PEQUEÑOS MAMIFEROS</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G73" s="4" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H73" s="4" t="n">
         <v>0</v>
@@ -18568,7 +18568,7 @@
         <v>0</v>
       </c>
       <c r="L73" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M73" s="5" t="n">
         <v>0</v>
@@ -18577,16 +18577,16 @@
         <v>0</v>
       </c>
       <c r="O73" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P73" s="4" t="n">
         <v>59</v>
       </c>
       <c r="Q73" s="4" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R73" s="4" t="n">
-        <v>190</v>
+        <v>393.33</v>
       </c>
       <c r="S73" s="5" t="n">
         <v>30</v>
@@ -18598,12 +18598,12 @@
       </c>
       <c r="U73" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 3.54€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V73" s="4" t="inlineStr">
         <is>
-          <t>Compra 02/01/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W73" s="4" t="inlineStr">
@@ -18615,24 +18615,32 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>2707190007</t>
+          <t>2806030001</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>PANAQUE MAMLUS L104</t>
-        </is>
-      </c>
-      <c r="C74" s="3" t="inlineStr"/>
-      <c r="D74" s="3" t="inlineStr"/>
+          <t>COMETA SURTIDO XXL</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>15CM</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E74" s="4" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>2806</t>
         </is>
       </c>
       <c r="F74" s="4" t="inlineStr">
         <is>
-          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
+          <t>PECES JARDIN ACUATICO</t>
         </is>
       </c>
       <c r="G74" s="4" t="n">
@@ -18651,7 +18659,7 @@
         <v>0</v>
       </c>
       <c r="L74" s="4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M74" s="5" t="n">
         <v>0</v>
@@ -18660,7 +18668,7 @@
         <v>0</v>
       </c>
       <c r="O74" s="4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P74" s="4" t="n">
         <v>59</v>
@@ -18681,7 +18689,7 @@
       </c>
       <c r="U74" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 21.39€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.22€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V74" s="4" t="inlineStr">
@@ -18698,32 +18706,24 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>2705040004</t>
+          <t>2707070003</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>PLANTAS EN TRONCO</t>
-        </is>
-      </c>
-      <c r="C75" s="3" t="inlineStr">
-        <is>
-          <t>3UD</t>
-        </is>
-      </c>
-      <c r="D75" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>TETRA PRISTELLA ROJA INIRIDA</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="inlineStr"/>
+      <c r="D75" s="3" t="inlineStr"/>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F75" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G75" s="4" t="n">
@@ -18742,7 +18742,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="4" t="n">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="M75" s="5" t="n">
         <v>0</v>
@@ -18751,7 +18751,7 @@
         <v>0</v>
       </c>
       <c r="O75" s="4" t="n">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="P75" s="4" t="n">
         <v>59</v>
@@ -18772,7 +18772,7 @@
       </c>
       <c r="U75" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 12.35€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 44.1€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V75" s="4" t="inlineStr">
@@ -18789,24 +18789,24 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>2705040003</t>
+          <t>2707110022</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA XL</t>
+          <t>CORYDORA ORANGE VENEZUELA</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr"/>
       <c r="D76" s="3" t="inlineStr"/>
       <c r="E76" s="4" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="F76" s="4" t="inlineStr">
         <is>
-          <t>PLANTA ACUATICA DECORACION ACUARIOFILIA</t>
+          <t>PECES AGUA CALIENTE ACUARIOFILIA</t>
         </is>
       </c>
       <c r="G76" s="4" t="n">
@@ -18825,7 +18825,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M76" s="5" t="n">
         <v>0</v>
@@ -18834,7 +18834,7 @@
         <v>0</v>
       </c>
       <c r="O76" s="4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P76" s="4" t="n">
         <v>59</v>
@@ -18855,7 +18855,7 @@
       </c>
       <c r="U76" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 14.29€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 9.58€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V76" s="4" t="inlineStr">
@@ -18872,12 +18872,12 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>2707110005</t>
+          <t>2707100004</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>BOTIA MORLETI 4</t>
+          <t>APISTOGRAMA CACATUOIDES</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr"/>
@@ -18908,7 +18908,7 @@
         <v>0</v>
       </c>
       <c r="L77" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M77" s="5" t="n">
         <v>0</v>
@@ -18917,7 +18917,7 @@
         <v>0</v>
       </c>
       <c r="O77" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P77" s="4" t="n">
         <v>59</v>
@@ -18938,7 +18938,7 @@
       </c>
       <c r="U77" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.31€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 30% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 2.79€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V77" s="4" t="inlineStr">

</xml_diff>